<commit_message>
finalise fig 1 sheet genus
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="988" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2B6E93EC-4755-4F81-BFBC-2CC1FE153478}"/>
+  <xr:revisionPtr revIDLastSave="992" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4E6444F4-94F6-488E-BBDA-030A4C21E860}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,16 @@
     <sheet name="species" sheetId="4" r:id="rId5"/>
     <sheet name="spec per gen" sheetId="8" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">genus!$D$2:$E$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AE$390</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
-    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -3152,8 +3149,8 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7BB13960-1F10-4A06-88AF-4B19BB9057A6}" type="CELLRANGE">
-                      <a:rPr lang="en-US"/>
+                    <a:fld id="{737BA9E9-8BB7-46C3-9D38-13DE5B08ECBD}" type="CELLRANGE">
+                      <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
                     </a:fld>
@@ -3161,6 +3158,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3170,6 +3168,7 @@
               <c:extLst>
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
@@ -3184,7 +3183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{91B59F98-6CF4-4A9E-9247-AEC72256B762}" type="CELLRANGE">
+                    <a:fld id="{6045CAFA-7B8B-4E2A-8BD5-0424545FE6F9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3193,6 +3192,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3217,7 +3217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D500D0C-99E3-4EF7-ABDA-03B988C1F618}" type="CELLRANGE">
+                    <a:fld id="{D85AEA1A-2E2B-4F1E-9C2A-CBCCCF8DD924}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3226,6 +3226,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3250,7 +3251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2490FB05-7D99-4BB3-A6C1-D3C4CF4F9B16}" type="CELLRANGE">
+                    <a:fld id="{70146ABA-E85C-40AB-87CA-3FB7AA49A94D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3259,6 +3260,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3283,7 +3285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B74FDE21-7DF3-44CF-97D3-CFA27E8F8BC3}" type="CELLRANGE">
+                    <a:fld id="{FAF81016-A379-478C-952F-521CAFE7889C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3292,6 +3294,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3316,7 +3319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{59E405F3-B231-4369-8EFB-6E9BA3009E7A}" type="CELLRANGE">
+                    <a:fld id="{EEB111A0-C462-4A46-BD94-9400EE961060}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3325,6 +3328,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3349,7 +3353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9DCD22D7-A035-46E3-A7F5-A85EAF68FFF5}" type="CELLRANGE">
+                    <a:fld id="{F480C7F8-0ECA-4B61-A7A1-322D0495F1FD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3358,6 +3362,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3382,7 +3387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{89F2DE69-EA6F-4771-BDE1-548A24AB7BCA}" type="CELLRANGE">
+                    <a:fld id="{C5072ACC-0573-44F6-8553-C30538598129}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3391,6 +3396,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3415,7 +3421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4E2ACA97-0187-4689-BE27-FD35033A4B9D}" type="CELLRANGE">
+                    <a:fld id="{84A03DA5-6CC7-4F9F-B4FF-3DFE5CF6C2C8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3424,6 +3430,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3448,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7D3E57D6-9768-4A31-9C95-49E638EA1B16}" type="CELLRANGE">
+                    <a:fld id="{7BA5F0D4-CF04-44D3-90BE-DF6231B3B1C4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3457,6 +3464,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3481,7 +3489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3600BC93-0F08-4E6F-B5BA-C0E17C7CF885}" type="CELLRANGE">
+                    <a:fld id="{C42891CB-E5DD-4B88-816F-42FA38BAB562}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3490,6 +3498,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3514,7 +3523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D516DE00-8F96-4A56-9657-A7BF183279F8}" type="CELLRANGE">
+                    <a:fld id="{469CCCAD-3FA0-4F6D-9922-42F25E49A631}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3523,6 +3532,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3547,7 +3557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A432A786-7908-4B75-8BB5-55C2A8DFA431}" type="CELLRANGE">
+                    <a:fld id="{1602270D-B931-48B1-8186-42EDE6C124C1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3556,6 +3566,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3580,7 +3591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{089E5030-32AA-4274-8EDB-4CC79C28A282}" type="CELLRANGE">
+                    <a:fld id="{B3CAB7B9-F48E-4201-A77A-1326BD59FD57}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3589,6 +3600,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3613,7 +3625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{22C58E9E-2486-4347-966B-EB54F9C7590D}" type="CELLRANGE">
+                    <a:fld id="{20151A2B-730E-45C8-9348-250C05417CDA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3622,6 +3634,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3646,7 +3659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19024968-43CE-4871-82D6-F3018AE54AD2}" type="CELLRANGE">
+                    <a:fld id="{A110118B-80B1-4114-A017-CEA36A8B358F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3655,6 +3668,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3679,7 +3693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0DC25C4C-69FB-48ED-94FB-99EBBCF7B865}" type="CELLRANGE">
+                    <a:fld id="{3A87ED28-4B36-42DC-BDE0-A6E7D6A4ACB0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3688,6 +3702,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3712,7 +3727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9CA0EC46-1AB3-478C-A5F1-DF30C171EDED}" type="CELLRANGE">
+                    <a:fld id="{5A5C4FF8-2CAC-4E0E-AB28-4E5D619C1F8D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3721,6 +3736,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3745,7 +3761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3595D717-8855-4082-8A37-D02992EC3341}" type="CELLRANGE">
+                    <a:fld id="{57CC1606-CB11-4937-8DEF-A6947F6CE747}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3754,6 +3770,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3778,7 +3795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2F284878-9288-4744-80D3-7EA8E6C9BE14}" type="CELLRANGE">
+                    <a:fld id="{EADF7C37-381B-41B7-889E-679A52453D66}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3787,6 +3804,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3811,7 +3829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C3A37891-6B1B-4775-B4B3-474F982476C3}" type="CELLRANGE">
+                    <a:fld id="{74A66E97-BFE5-458F-A240-16051FD9DB6A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3820,6 +3838,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3844,7 +3863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6D24742A-6134-4DE4-9765-322F513EEE06}" type="CELLRANGE">
+                    <a:fld id="{CEC67707-737B-4016-9956-2520913DC21F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3853,6 +3872,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3877,7 +3897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C86060E5-7E2E-4B4F-9652-0EBD51D16F3A}" type="CELLRANGE">
+                    <a:fld id="{6E886F40-93B7-4C4C-A481-A8C2FB1E5B51}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3886,6 +3906,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3910,7 +3931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E9D45385-49D0-4C71-950E-5BC0F487B691}" type="CELLRANGE">
+                    <a:fld id="{52051019-F576-43C3-9BE0-B1197F9D9BC6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3919,6 +3940,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3943,7 +3965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EB01175E-243D-451D-A286-D8A121F7940F}" type="CELLRANGE">
+                    <a:fld id="{482EB67B-EF86-4FCB-ACB6-C0B8713F6E2B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3952,6 +3974,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -3976,7 +3999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{781E243E-DB30-4D07-84E7-7248F498958A}" type="CELLRANGE">
+                    <a:fld id="{51E25A61-905D-4281-A3B6-EE0843904F23}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3985,6 +4008,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4009,7 +4033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7F780043-A253-441B-84D5-098393916ADC}" type="CELLRANGE">
+                    <a:fld id="{EC06D55D-AA6B-4CE0-900B-7CCEB816468B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4018,6 +4042,7 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:dLblPos val="outEnd"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
               <c:showCatName val="0"/>
@@ -4036,9 +4061,42 @@
               </c:extLst>
             </c:dLbl>
             <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
+              <a:solidFill>
+                <a:schemeClr val="bg1">
+                  <a:alpha val="48000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln cap="flat">
+                <a:gradFill flip="none" rotWithShape="1">
+                  <a:gsLst>
+                    <a:gs pos="0">
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="5000"/>
+                        <a:lumOff val="95000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="74000">
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="45000"/>
+                        <a:lumOff val="55000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="83000">
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="45000"/>
+                        <a:lumOff val="55000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                    <a:gs pos="100000">
+                      <a:schemeClr val="accent3">
+                        <a:lumMod val="30000"/>
+                        <a:lumOff val="70000"/>
+                      </a:schemeClr>
+                    </a:gs>
+                  </a:gsLst>
+                  <a:lin ang="5400000" scaled="1"/>
+                  <a:tileRect/>
+                </a:gradFill>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
@@ -4064,6 +4122,7 @@
                 <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="outEnd"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -4264,7 +4323,7 @@
                 <c15:dlblRangeCache>
                   <c:ptCount val="27"/>
                   <c:pt idx="0">
-                    <c:v>9</c:v>
+                    <c:v>11</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>6</c:v>
@@ -4303,7 +4362,7 @@
                     <c:v>1</c:v>
                   </c:pt>
                   <c:pt idx="13">
-                    <c:v>1</c:v>
+                    <c:v>2</c:v>
                   </c:pt>
                   <c:pt idx="14">
                     <c:v>2</c:v>
@@ -7875,12 +7934,12 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>205740</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -7949,21 +8008,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12898,14 +12942,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF390"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AG1048576"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -47579,8 +47623,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6336F052-340A-4111-968E-001D4CF7123D}">
   <dimension ref="A1:J61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O27" sqref="O27"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47632,7 +47676,7 @@
         <v>24.164524421593832</v>
       </c>
       <c r="I2" s="5">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -47970,7 +48014,7 @@
         <v>91.516709511568124</v>
       </c>
       <c r="I15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
start rationale data paper
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1012" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{C2B136DC-901F-474B-B28F-7615429CC6E7}"/>
+  <xr:revisionPtr revIDLastSave="1013" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4F4301F6-F61D-47DF-A367-8C3B9A7972C2}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3149,7 +3149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{851A30BF-AF01-4D4E-BDEA-42BA6C3C5793}" type="CELLRANGE">
+                    <a:fld id="{79BD6500-A27B-42EF-B372-FBC7D3BE8C48}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3183,7 +3183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{328AC28E-301F-4E00-A55D-4CBF505FCA09}" type="CELLRANGE">
+                    <a:fld id="{514240D0-AE77-4091-ADBE-F3655BD8A223}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3217,7 +3217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{76DAE307-AA29-4ED3-A476-5C5B6C0B8445}" type="CELLRANGE">
+                    <a:fld id="{B2DAF998-51CB-43BA-BABD-0C3157EE2036}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3251,7 +3251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BC5D0FB6-30E1-4A7D-A638-436BF6448DBD}" type="CELLRANGE">
+                    <a:fld id="{3DB4137A-96DF-407A-AA09-671377CD8ED7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3285,7 +3285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6428539B-C40F-4F5C-B1AF-2D5060E0E9BF}" type="CELLRANGE">
+                    <a:fld id="{D78B2E88-ADE9-4F02-9F3C-7DBB393C8565}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3319,7 +3319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37FFCF71-00FF-4766-8D1F-B6B0BBD92DB0}" type="CELLRANGE">
+                    <a:fld id="{B2AACDDF-20E2-47EA-B023-9A6902D74A92}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3353,7 +3353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{ABBBC013-F374-4D5D-A4C0-CA02F263093D}" type="CELLRANGE">
+                    <a:fld id="{118C41E7-6473-4DA0-A99F-98C4B41C2AD2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3387,7 +3387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E84CBA4-DB56-4F38-A0B7-C73F54DF738A}" type="CELLRANGE">
+                    <a:fld id="{177F633F-60C5-4D76-86BE-CEE00038DAB8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3421,7 +3421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7571297A-6F18-408F-8A92-433DC00669F1}" type="CELLRANGE">
+                    <a:fld id="{C06A0F28-1B82-4B56-B9F1-C61633DA7101}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3455,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FB510219-15B6-4481-949E-929870D4D770}" type="CELLRANGE">
+                    <a:fld id="{8B26A108-181F-445E-9B85-1601038B2257}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3489,7 +3489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5261C4CB-BE37-4E1F-9763-521AAD78B752}" type="CELLRANGE">
+                    <a:fld id="{1C346592-BD75-417A-974C-7B9E41C47D18}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3523,7 +3523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2C7CAC03-78C4-4F70-A333-EBD8ACC886F3}" type="CELLRANGE">
+                    <a:fld id="{F97409B1-B0E5-4E34-887E-02A99A8D59FD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3557,7 +3557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{28BAFD06-3150-435B-8D8D-20811D3DD231}" type="CELLRANGE">
+                    <a:fld id="{A50C7454-7DA2-4198-BA8E-4B3A7AC6A4CD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3591,7 +3591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{054BA77F-DE7F-4702-B1C2-171C6D117A80}" type="CELLRANGE">
+                    <a:fld id="{FC2E05ED-D4D7-432B-9753-5D3EC7A29E99}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3625,7 +3625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6DD612BD-197A-40E1-839E-2E8A932941EB}" type="CELLRANGE">
+                    <a:fld id="{C16CF261-FFAD-4E29-BF53-E112043584ED}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3659,7 +3659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2CFDA3AB-A490-47EE-9DAF-6917EC9BC0EB}" type="CELLRANGE">
+                    <a:fld id="{74BBA585-CE48-4A16-AEE3-71E9DB83106F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3693,7 +3693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DC7FBACD-7870-4CC7-AEE3-08631E9AFD06}" type="CELLRANGE">
+                    <a:fld id="{296979B9-13CC-456B-83BB-48C751C8467C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3727,7 +3727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1F2C434B-112E-4789-8D35-E55C6087160F}" type="CELLRANGE">
+                    <a:fld id="{1BBCEC12-64E8-4FDC-8A42-034EBDF41208}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3761,7 +3761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CD774B74-6F37-4F29-9982-B3C9FBC5E1C4}" type="CELLRANGE">
+                    <a:fld id="{6843AC25-80A8-409E-B0AC-2EED850FC417}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3795,7 +3795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3FB0439-1105-4342-928F-8D8C34D76F5C}" type="CELLRANGE">
+                    <a:fld id="{4FF99E03-1FA3-40CD-BA7A-41A3A0D961FA}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3829,7 +3829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0F02091-E01C-46B8-BE52-C3475E8D1AB5}" type="CELLRANGE">
+                    <a:fld id="{5F17B63D-2C89-4BCF-97D7-743373F5DE9B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3863,7 +3863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{671C68FC-D626-4913-B7E5-E872DCB8B1E7}" type="CELLRANGE">
+                    <a:fld id="{F8990689-E5DD-491F-AE30-8FC5FEA50F5E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3897,7 +3897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B66EDB78-4753-4F19-83B4-C2D435C294EE}" type="CELLRANGE">
+                    <a:fld id="{4E1D0A16-14A9-477A-ACD2-B3FD90FB4A34}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3931,7 +3931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D0532308-60DE-4FA4-BDF2-FAE6A8CFE8FC}" type="CELLRANGE">
+                    <a:fld id="{46AF5032-3C6C-4900-84DF-32A9CCE9D645}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3965,7 +3965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FE9C9D7B-6CAB-4FC5-94A5-EC1242681D7F}" type="CELLRANGE">
+                    <a:fld id="{EA05FDB7-7107-471C-9A72-3D42D45A2794}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3999,7 +3999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FC95A477-0D64-4FB3-8D47-4F49CBCBFC2C}" type="CELLRANGE">
+                    <a:fld id="{4EAC9B82-3237-427E-9659-252226BBE72A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4033,7 +4033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{179B1C53-F31A-441D-818F-0BFAA739D3E5}" type="CELLRANGE">
+                    <a:fld id="{7F7675F2-3636-4316-BFAB-372D795B85F8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5057,7 +5057,7 @@
               <c:strCache>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>Monilearia persimilis</c:v>
+                  <c:v>Monilearia spec.</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Caracollina lenticula</c:v>
@@ -5494,7 +5494,7 @@
               <c:strCache>
                 <c:ptCount val="62"/>
                 <c:pt idx="0">
-                  <c:v>Monilearia persimilis</c:v>
+                  <c:v>Monilearia spec.</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>Caracollina lenticula</c:v>
@@ -12942,7 +12942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="T1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="AD4" sqref="AD4"/>
     </sheetView>
   </sheetViews>
@@ -46827,7 +46827,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I28" sqref="I28"/>
+      <selection activeCell="E2" sqref="E2:E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -47366,7 +47366,7 @@
   <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="T11" sqref="T11"/>
+      <selection activeCell="D2" sqref="D2:D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48239,8 +48239,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F610DE0-7E1E-45E0-A6B7-F8E58D926A48}">
   <dimension ref="A1:H67"/>
   <sheetViews>
-    <sheetView topLeftCell="A40" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="U20" sqref="U20"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D63" sqref="D2:D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -48271,7 +48271,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D2" s="1" t="s">
-        <v>145</v>
+        <v>723</v>
       </c>
       <c r="E2" s="1">
         <v>43</v>

</xml_diff>

<commit_message>
final update correct quantities
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1025" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{969CD0D9-8373-45EB-BD49-011BC07D71F6}"/>
+  <xr:revisionPtr revIDLastSave="1175" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{2CA95A30-7708-49F1-9F75-26FC3CF8997F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8378" uniqueCount="727">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8380" uniqueCount="727">
   <si>
     <t>orderNumber</t>
   </si>
@@ -3149,7 +3149,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0CB9F2D1-B0D8-4E9E-B4F8-09BA4328AE91}" type="CELLRANGE">
+                    <a:fld id="{BBAC1227-3A4F-4816-89B9-69B546C312AC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3183,7 +3183,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{19906340-45A8-449C-8963-06F99A460C86}" type="CELLRANGE">
+                    <a:fld id="{B0BAB484-596C-429A-B04A-94CAD3B3E5F0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3217,7 +3217,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8D2E5EC-FCF7-4673-BC31-251EF141C8AF}" type="CELLRANGE">
+                    <a:fld id="{AE8053EA-F7EC-467D-9C0B-456AC412105D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3251,7 +3251,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B22842E9-9543-4D4E-BBF4-D044C2F8ECF9}" type="CELLRANGE">
+                    <a:fld id="{22F73173-94B5-4ED9-9462-7C1A2A9ED117}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3285,7 +3285,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6FDEC09B-5422-4B26-8D5C-C31CAA569546}" type="CELLRANGE">
+                    <a:fld id="{43DD36A9-8774-48C1-9E6B-A43703E3E395}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3319,7 +3319,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E7F6A7D1-6F30-474D-ACA1-6DB33C67164E}" type="CELLRANGE">
+                    <a:fld id="{67FB98BE-E564-40CC-A77B-2DE31FD5A09E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3353,7 +3353,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAC7B0A1-E245-489A-9ADF-D784CD038881}" type="CELLRANGE">
+                    <a:fld id="{6E8CD749-4FAE-4D71-87B6-851DA2344764}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3387,7 +3387,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{41DACEB7-F275-48F0-B1C6-15D3505D03E2}" type="CELLRANGE">
+                    <a:fld id="{67179E68-A0A4-47AD-850E-C8D608E66C0D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3421,7 +3421,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A3FC0286-494F-4310-A36D-BF767D9D52C7}" type="CELLRANGE">
+                    <a:fld id="{CC083820-5F97-4734-8494-C6C8BD0ABAAC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3455,7 +3455,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D469F7E3-5B3E-454B-9598-4768D70B95B7}" type="CELLRANGE">
+                    <a:fld id="{EA22A2AE-FEA8-41A6-AEAE-E985AFFBC783}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3489,7 +3489,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{849A302A-473C-4892-A92A-CCDF54CB15A1}" type="CELLRANGE">
+                    <a:fld id="{EA168306-4B2D-4851-828B-9585391CD751}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3523,7 +3523,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2671249C-8ADD-4BDF-952B-4F6B8FDA8247}" type="CELLRANGE">
+                    <a:fld id="{C20958ED-AB44-4EB9-94E4-99ADF286633C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3557,7 +3557,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B8C3134A-F11E-40D0-BD52-D3FCBDC6FEC1}" type="CELLRANGE">
+                    <a:fld id="{4807AF11-5994-40A0-A03D-2CB20A1D783B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3591,7 +3591,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7144B0AE-19A1-4020-BD24-E7075B9955CA}" type="CELLRANGE">
+                    <a:fld id="{74798F79-4E0C-4B8D-9B3A-BAD9B05F65B5}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3625,7 +3625,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3AC1346-E7A4-4287-95AA-704E5376BC6F}" type="CELLRANGE">
+                    <a:fld id="{3F535523-D27B-40F7-9621-D947838AFE61}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3659,7 +3659,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0A85D4DE-54AC-4427-BE9C-AF7EF529A8FA}" type="CELLRANGE">
+                    <a:fld id="{C392FB46-43D5-421B-85B6-37968AB3BF51}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3693,7 +3693,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AAF76FCF-A7B5-4A3C-9576-5AC95DED2FBD}" type="CELLRANGE">
+                    <a:fld id="{0B59470E-BBFC-48BC-9B9A-B600A1CEFF31}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3727,7 +3727,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EA2705CB-8EE2-4A05-AFE7-238024837FC5}" type="CELLRANGE">
+                    <a:fld id="{00124449-900B-4201-9927-D14F98DFBAFE}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3761,7 +3761,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{483E5FF7-14C8-41D3-9168-031280F7CD08}" type="CELLRANGE">
+                    <a:fld id="{77B92C2C-E711-4323-9D4F-EE0152DC68B9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3795,7 +3795,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{32963CAE-48BE-49D0-9428-E2C1C7D617AE}" type="CELLRANGE">
+                    <a:fld id="{2636D492-0030-4412-9587-99E3711AB298}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3829,7 +3829,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{1A75239B-422B-4589-B37E-E78E3D78CFB2}" type="CELLRANGE">
+                    <a:fld id="{C08D20E9-75AA-47C9-96EC-6FFD09CDF08A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3863,7 +3863,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D897EF7A-B34C-4926-BC79-9E107695A0C0}" type="CELLRANGE">
+                    <a:fld id="{D4D42960-0A53-4969-A262-E539716A6970}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3897,7 +3897,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A6744963-9F60-40F2-9875-D60F7B564292}" type="CELLRANGE">
+                    <a:fld id="{A3D9EABD-EF7B-4F5A-AC4B-53C0429910B5}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3931,7 +3931,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{962D4A3F-3664-48F2-A16F-8049A0AD6798}" type="CELLRANGE">
+                    <a:fld id="{19077D00-2614-4265-A571-981F53C71ECD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3965,7 +3965,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D8869FB9-D526-4B05-B1AE-BD38A6F97123}" type="CELLRANGE">
+                    <a:fld id="{CF707652-00FC-4384-ADE8-35CC01830357}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3999,7 +3999,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{37A49B65-117A-4C1F-960B-D664C3889999}" type="CELLRANGE">
+                    <a:fld id="{587B81C7-9417-4878-BAD5-19E11917A3A0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4033,7 +4033,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{20233F7C-B8C7-4E2A-BCBB-977F1D83D3F1}" type="CELLRANGE">
+                    <a:fld id="{A3F25F79-DBE2-4115-BE17-2C9E9830712F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -12942,8 +12942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="AE177" sqref="AE53:AE177"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Q385" sqref="Q385"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14699,6 +14699,9 @@
       <c r="L21" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N21" s="1">
+        <v>20</v>
+      </c>
       <c r="O21" s="1" t="s">
         <v>639</v>
       </c>
@@ -14779,6 +14782,9 @@
       <c r="L22" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N22" s="1">
+        <v>20</v>
+      </c>
       <c r="O22" s="1" t="s">
         <v>639</v>
       </c>
@@ -15035,7 +15041,7 @@
         <v>643</v>
       </c>
       <c r="N25" s="1">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="O25" s="1" t="s">
         <v>640</v>
@@ -15375,6 +15381,9 @@
       <c r="L29" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N29" s="1">
+        <v>20</v>
+      </c>
       <c r="O29" s="1" t="s">
         <v>639</v>
       </c>
@@ -15799,6 +15808,9 @@
       <c r="L34" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N34" s="1">
+        <v>20</v>
+      </c>
       <c r="O34" s="1" t="s">
         <v>639</v>
       </c>
@@ -16054,6 +16066,9 @@
       <c r="L37" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N37" s="1">
+        <v>50</v>
+      </c>
       <c r="O37" s="1" t="s">
         <v>639</v>
       </c>
@@ -16134,6 +16149,9 @@
       <c r="L38" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N38" s="1">
+        <v>20</v>
+      </c>
       <c r="O38" s="1" t="s">
         <v>639</v>
       </c>
@@ -17195,6 +17213,9 @@
       <c r="L51" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N51" s="1">
+        <v>30</v>
+      </c>
       <c r="O51" s="1" t="s">
         <v>639</v>
       </c>
@@ -17269,6 +17290,9 @@
       <c r="L52" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N52" s="1">
+        <v>40</v>
+      </c>
       <c r="O52" s="1" t="s">
         <v>639</v>
       </c>
@@ -17441,6 +17465,9 @@
       <c r="L54" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N54" s="1">
+        <v>20</v>
+      </c>
       <c r="O54" s="1" t="s">
         <v>639</v>
       </c>
@@ -18037,6 +18064,9 @@
       <c r="L61" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N61" s="1">
+        <v>30</v>
+      </c>
       <c r="O61" s="1" t="s">
         <v>639</v>
       </c>
@@ -18553,6 +18583,9 @@
       <c r="L67" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N67" s="1">
+        <v>30</v>
+      </c>
       <c r="O67" s="1" t="s">
         <v>639</v>
       </c>
@@ -18719,6 +18752,9 @@
       <c r="L69" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N69" s="1">
+        <v>30</v>
+      </c>
       <c r="O69" s="1" t="s">
         <v>639</v>
       </c>
@@ -18799,6 +18835,9 @@
       <c r="L70" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N70" s="1">
+        <v>50</v>
+      </c>
       <c r="O70" s="1" t="s">
         <v>639</v>
       </c>
@@ -18879,6 +18918,9 @@
       <c r="L71" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N71" s="1">
+        <v>50</v>
+      </c>
       <c r="O71" s="1" t="s">
         <v>639</v>
       </c>
@@ -19045,6 +19087,9 @@
       <c r="L73" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N73" s="1">
+        <v>50</v>
+      </c>
       <c r="O73" s="1" t="s">
         <v>639</v>
       </c>
@@ -19386,6 +19431,9 @@
       <c r="L77" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N77" s="1">
+        <v>25</v>
+      </c>
       <c r="O77" s="1" t="s">
         <v>639</v>
       </c>
@@ -21338,6 +21386,9 @@
       <c r="L101" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N101" s="1">
+        <v>20</v>
+      </c>
       <c r="O101" s="1" t="s">
         <v>639</v>
       </c>
@@ -23361,6 +23412,9 @@
       <c r="L126" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N126" s="1">
+        <v>20</v>
+      </c>
       <c r="O126" s="1" t="s">
         <v>639</v>
       </c>
@@ -23527,6 +23581,9 @@
       <c r="L128" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N128" s="1">
+        <v>40</v>
+      </c>
       <c r="O128" s="1" t="s">
         <v>639</v>
       </c>
@@ -24132,6 +24189,9 @@
       <c r="L135" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N135" s="1">
+        <v>20</v>
+      </c>
       <c r="O135" s="1" t="s">
         <v>639</v>
       </c>
@@ -24212,6 +24272,9 @@
       <c r="L136" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N136" s="1">
+        <v>25</v>
+      </c>
       <c r="O136" s="1" t="s">
         <v>639</v>
       </c>
@@ -24292,6 +24355,9 @@
       <c r="L137" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N137" s="1">
+        <v>10</v>
+      </c>
       <c r="O137" s="1" t="s">
         <v>639</v>
       </c>
@@ -25226,6 +25292,9 @@
       <c r="L148" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N148" s="1">
+        <v>30</v>
+      </c>
       <c r="O148" s="1" t="s">
         <v>639</v>
       </c>
@@ -26172,6 +26241,9 @@
       <c r="L159" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N159" s="1">
+        <v>40</v>
+      </c>
       <c r="O159" s="1" t="s">
         <v>639</v>
       </c>
@@ -28984,6 +29056,9 @@
       <c r="L191" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N191" s="1">
+        <v>40</v>
+      </c>
       <c r="O191" s="1" t="s">
         <v>639</v>
       </c>
@@ -29334,6 +29409,9 @@
       <c r="L195" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N195" s="1">
+        <v>10</v>
+      </c>
       <c r="O195" s="1" t="s">
         <v>639</v>
       </c>
@@ -29420,6 +29498,9 @@
       <c r="L196" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N196" s="1">
+        <v>50</v>
+      </c>
       <c r="O196" s="1" t="s">
         <v>639</v>
       </c>
@@ -29681,6 +29762,9 @@
       <c r="L199" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N199" s="1">
+        <v>9</v>
+      </c>
       <c r="O199" s="1" t="s">
         <v>640</v>
       </c>
@@ -29758,6 +29842,9 @@
       <c r="L200" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N200" s="1">
+        <v>1</v>
+      </c>
       <c r="O200" s="1" t="s">
         <v>640</v>
       </c>
@@ -29838,6 +29925,9 @@
       <c r="L201" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N201" s="1">
+        <v>1</v>
+      </c>
       <c r="O201" s="1" t="s">
         <v>640</v>
       </c>
@@ -29909,6 +29999,9 @@
       <c r="L202" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N202" s="1">
+        <v>4</v>
+      </c>
       <c r="O202" s="1" t="s">
         <v>640</v>
       </c>
@@ -30075,6 +30168,9 @@
       <c r="L204" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N204" s="1">
+        <v>10</v>
+      </c>
       <c r="O204" s="1" t="s">
         <v>640</v>
       </c>
@@ -30152,6 +30248,9 @@
       <c r="L205" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N205" s="1">
+        <v>10</v>
+      </c>
       <c r="O205" s="1" t="s">
         <v>640</v>
       </c>
@@ -30407,6 +30506,9 @@
       <c r="L208" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N208" s="1">
+        <v>15</v>
+      </c>
       <c r="O208" s="1" t="s">
         <v>639</v>
       </c>
@@ -30493,6 +30595,9 @@
       <c r="L209" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N209" s="1">
+        <v>40</v>
+      </c>
       <c r="O209" s="1" t="s">
         <v>639</v>
       </c>
@@ -30571,6 +30676,9 @@
       <c r="L210" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N210" s="1">
+        <v>20</v>
+      </c>
       <c r="O210" s="1" t="s">
         <v>639</v>
       </c>
@@ -30746,6 +30854,9 @@
       <c r="L212" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N212" s="1">
+        <v>40</v>
+      </c>
       <c r="O212" s="1" t="s">
         <v>639</v>
       </c>
@@ -31010,6 +31121,9 @@
       <c r="L215" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N215" s="1">
+        <v>15</v>
+      </c>
       <c r="O215" s="1" t="s">
         <v>639</v>
       </c>
@@ -31096,6 +31210,9 @@
       <c r="L216" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N216" s="1">
+        <v>50</v>
+      </c>
       <c r="O216" s="1" t="s">
         <v>639</v>
       </c>
@@ -31333,6 +31450,9 @@
       <c r="L219" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N219" s="1">
+        <v>20</v>
+      </c>
       <c r="O219" s="1" t="s">
         <v>639</v>
       </c>
@@ -31422,6 +31542,9 @@
       <c r="L220" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N220" s="1">
+        <v>50</v>
+      </c>
       <c r="O220" s="1" t="s">
         <v>639</v>
       </c>
@@ -31505,6 +31628,9 @@
       <c r="L221" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N221" s="1">
+        <v>30</v>
+      </c>
       <c r="O221" s="1" t="s">
         <v>639</v>
       </c>
@@ -31591,6 +31717,9 @@
       <c r="L222" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N222" s="1">
+        <v>15</v>
+      </c>
       <c r="O222" s="1" t="s">
         <v>639</v>
       </c>
@@ -31674,6 +31803,9 @@
       <c r="L223" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N223" s="1">
+        <v>10</v>
+      </c>
       <c r="O223" s="1" t="s">
         <v>639</v>
       </c>
@@ -31920,6 +32052,9 @@
       <c r="L226" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N226" s="1">
+        <v>10</v>
+      </c>
       <c r="O226" s="1" t="s">
         <v>639</v>
       </c>
@@ -32000,6 +32135,9 @@
       <c r="L227" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N227" s="1">
+        <v>10</v>
+      </c>
       <c r="O227" s="1" t="s">
         <v>639</v>
       </c>
@@ -32258,6 +32396,9 @@
       <c r="L230" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N230" s="1">
+        <v>1</v>
+      </c>
       <c r="O230" s="1" t="s">
         <v>640</v>
       </c>
@@ -32338,8 +32479,11 @@
       <c r="L231" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N231" s="1">
+        <v>5</v>
+      </c>
       <c r="O231" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P231" s="1">
         <v>27.888126373291001</v>
@@ -32409,6 +32553,9 @@
       <c r="L232" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N232" s="1">
+        <v>10</v>
+      </c>
       <c r="O232" s="1" t="s">
         <v>639</v>
       </c>
@@ -32489,6 +32636,9 @@
       <c r="L233" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N233" s="1">
+        <v>10</v>
+      </c>
       <c r="O233" s="1" t="s">
         <v>639</v>
       </c>
@@ -32566,6 +32716,9 @@
       <c r="L234" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N234" s="1">
+        <v>2</v>
+      </c>
       <c r="O234" s="1" t="s">
         <v>640</v>
       </c>
@@ -32652,6 +32805,9 @@
       <c r="L235" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N235" s="1">
+        <v>40</v>
+      </c>
       <c r="O235" s="1" t="s">
         <v>639</v>
       </c>
@@ -33085,6 +33241,9 @@
       <c r="L240" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N240" s="1">
+        <v>10</v>
+      </c>
       <c r="O240" s="1" t="s">
         <v>639</v>
       </c>
@@ -33165,6 +33324,9 @@
       <c r="L241" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N241" s="1">
+        <v>10</v>
+      </c>
       <c r="O241" s="1" t="s">
         <v>639</v>
       </c>
@@ -33420,6 +33582,9 @@
       <c r="L244" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N244" s="1">
+        <v>2</v>
+      </c>
       <c r="O244" s="1" t="s">
         <v>640</v>
       </c>
@@ -33503,6 +33668,9 @@
       <c r="L245" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N245" s="1">
+        <v>30</v>
+      </c>
       <c r="O245" s="1" t="s">
         <v>639</v>
       </c>
@@ -33580,6 +33748,9 @@
       <c r="L246" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N246" s="1">
+        <v>6</v>
+      </c>
       <c r="O246" s="1" t="s">
         <v>640</v>
       </c>
@@ -33755,6 +33926,9 @@
       <c r="L248" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N248" s="1">
+        <v>5</v>
+      </c>
       <c r="O248" s="1" t="s">
         <v>640</v>
       </c>
@@ -33838,6 +34012,9 @@
       <c r="L249" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N249" s="1">
+        <v>1</v>
+      </c>
       <c r="O249" s="1" t="s">
         <v>640</v>
       </c>
@@ -33915,6 +34092,9 @@
       <c r="L250" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N250" s="1">
+        <v>2</v>
+      </c>
       <c r="O250" s="1" t="s">
         <v>640</v>
       </c>
@@ -33992,6 +34172,9 @@
       <c r="L251" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N251" s="1">
+        <v>5</v>
+      </c>
       <c r="O251" s="1" t="s">
         <v>640</v>
       </c>
@@ -34072,8 +34255,11 @@
       <c r="L252" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N252" s="1">
+        <v>2</v>
+      </c>
       <c r="O252" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P252" s="1">
         <v>27.888401031494102</v>
@@ -34143,8 +34329,11 @@
       <c r="L253" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N253" s="1">
+        <v>2</v>
+      </c>
       <c r="O253" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P253" s="1">
         <v>27.8884162902832</v>
@@ -34223,6 +34412,9 @@
       <c r="L254" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N254" s="1">
+        <v>10</v>
+      </c>
       <c r="O254" s="1" t="s">
         <v>639</v>
       </c>
@@ -34309,6 +34501,9 @@
       <c r="L255" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N255" s="1">
+        <v>10</v>
+      </c>
       <c r="O255" s="1" t="s">
         <v>639</v>
       </c>
@@ -34386,6 +34581,9 @@
       <c r="L256" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N256" s="1">
+        <v>20</v>
+      </c>
       <c r="O256" s="1" t="s">
         <v>639</v>
       </c>
@@ -34650,6 +34848,9 @@
       <c r="L259" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N259" s="1">
+        <v>2</v>
+      </c>
       <c r="O259" s="1" t="s">
         <v>640</v>
       </c>
@@ -34908,6 +35109,9 @@
       <c r="L262" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N262" s="1">
+        <v>2</v>
+      </c>
       <c r="O262" s="1" t="s">
         <v>640</v>
       </c>
@@ -34988,6 +35192,9 @@
       <c r="L263" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N263" s="1">
+        <v>1</v>
+      </c>
       <c r="O263" s="1" t="s">
         <v>640</v>
       </c>
@@ -35060,6 +35267,9 @@
       <c r="L264" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N264" s="1">
+        <v>10</v>
+      </c>
       <c r="O264" s="1" t="s">
         <v>639</v>
       </c>
@@ -35140,6 +35350,9 @@
       <c r="L265" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N265" s="1">
+        <v>10</v>
+      </c>
       <c r="O265" s="1" t="s">
         <v>639</v>
       </c>
@@ -35212,6 +35425,9 @@
       <c r="L266" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N266" s="1">
+        <v>1</v>
+      </c>
       <c r="O266" s="1" t="s">
         <v>640</v>
       </c>
@@ -35292,6 +35508,9 @@
       <c r="L267" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N267" s="1">
+        <v>1</v>
+      </c>
       <c r="O267" s="1" t="s">
         <v>640</v>
       </c>
@@ -35373,6 +35592,9 @@
       <c r="L268" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N268" s="1">
+        <v>1</v>
+      </c>
       <c r="O268" s="1" t="s">
         <v>640</v>
       </c>
@@ -35542,6 +35764,9 @@
       <c r="L270" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N270" s="1">
+        <v>1</v>
+      </c>
       <c r="O270" s="1" t="s">
         <v>640</v>
       </c>
@@ -35622,6 +35847,9 @@
       <c r="L271" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N271" s="1">
+        <v>1</v>
+      </c>
       <c r="O271" s="1" t="s">
         <v>640</v>
       </c>
@@ -35699,6 +35927,9 @@
       <c r="L272" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N272" s="1">
+        <v>1</v>
+      </c>
       <c r="O272" s="1" t="s">
         <v>640</v>
       </c>
@@ -35776,6 +36007,9 @@
       <c r="L273" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N273" s="1">
+        <v>1</v>
+      </c>
       <c r="O273" s="1" t="s">
         <v>640</v>
       </c>
@@ -35853,6 +36087,9 @@
       <c r="L274" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N274" s="1">
+        <v>2</v>
+      </c>
       <c r="O274" s="1" t="s">
         <v>640</v>
       </c>
@@ -35933,6 +36170,9 @@
       <c r="L275" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N275" s="1">
+        <v>2</v>
+      </c>
       <c r="O275" s="1" t="s">
         <v>640</v>
       </c>
@@ -36004,6 +36244,9 @@
       <c r="L276" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N276" s="1">
+        <v>1</v>
+      </c>
       <c r="O276" s="1" t="s">
         <v>640</v>
       </c>
@@ -36087,6 +36330,9 @@
       <c r="L277" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N277" s="1">
+        <v>2</v>
+      </c>
       <c r="O277" s="1" t="s">
         <v>640</v>
       </c>
@@ -36167,6 +36413,9 @@
       <c r="L278" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N278" s="1">
+        <v>1</v>
+      </c>
       <c r="O278" s="1" t="s">
         <v>640</v>
       </c>
@@ -36247,6 +36496,9 @@
       <c r="L279" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N279" s="1">
+        <v>1</v>
+      </c>
       <c r="O279" s="1" t="s">
         <v>640</v>
       </c>
@@ -36327,6 +36579,9 @@
       <c r="L280" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N280" s="1">
+        <v>1</v>
+      </c>
       <c r="O280" s="1" t="s">
         <v>640</v>
       </c>
@@ -36404,6 +36659,9 @@
       <c r="L281" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N281" s="1">
+        <v>2</v>
+      </c>
       <c r="O281" s="1" t="s">
         <v>640</v>
       </c>
@@ -36482,6 +36740,9 @@
       <c r="L282" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N282" s="1">
+        <v>10</v>
+      </c>
       <c r="O282" s="1" t="s">
         <v>639</v>
       </c>
@@ -36563,6 +36824,9 @@
       <c r="L283" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N283" s="1">
+        <v>10</v>
+      </c>
       <c r="O283" s="1" t="s">
         <v>639</v>
       </c>
@@ -36635,6 +36899,9 @@
       <c r="L284" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N284" s="1">
+        <v>1</v>
+      </c>
       <c r="O284" s="1" t="s">
         <v>640</v>
       </c>
@@ -36718,6 +36985,9 @@
       <c r="L285" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N285" s="1">
+        <v>15</v>
+      </c>
       <c r="O285" s="1" t="s">
         <v>639</v>
       </c>
@@ -36796,6 +37066,9 @@
       <c r="L286" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N286" s="1">
+        <v>3</v>
+      </c>
       <c r="O286" s="1" t="s">
         <v>640</v>
       </c>
@@ -36868,8 +37141,11 @@
       <c r="L287" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N287" s="1">
+        <v>5</v>
+      </c>
       <c r="O287" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="P287" s="1">
         <v>27.894123077392599</v>
@@ -37037,6 +37313,9 @@
       <c r="L289" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N289" s="1">
+        <v>1</v>
+      </c>
       <c r="O289" s="1" t="s">
         <v>640</v>
       </c>
@@ -37117,6 +37396,9 @@
       <c r="L290" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N290" s="1">
+        <v>2</v>
+      </c>
       <c r="O290" s="1" t="s">
         <v>640</v>
       </c>
@@ -37194,6 +37476,9 @@
       <c r="L291" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N291" s="1">
+        <v>2</v>
+      </c>
       <c r="O291" s="1" t="s">
         <v>640</v>
       </c>
@@ -37265,6 +37550,9 @@
       <c r="L292" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N292" s="1">
+        <v>25</v>
+      </c>
       <c r="O292" s="1" t="s">
         <v>639</v>
       </c>
@@ -37523,6 +37811,9 @@
       <c r="L295" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N295" s="1">
+        <v>10</v>
+      </c>
       <c r="O295" s="1" t="s">
         <v>639</v>
       </c>
@@ -37781,6 +38072,9 @@
       <c r="L298" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N298" s="1">
+        <v>1</v>
+      </c>
       <c r="O298" s="1" t="s">
         <v>640</v>
       </c>
@@ -37852,6 +38146,9 @@
       <c r="L299" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N299" s="1">
+        <v>10</v>
+      </c>
       <c r="O299" s="1" t="s">
         <v>639</v>
       </c>
@@ -38009,6 +38306,9 @@
       <c r="L301" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N301" s="1">
+        <v>1</v>
+      </c>
       <c r="O301" s="1" t="s">
         <v>640</v>
       </c>
@@ -38178,6 +38478,9 @@
       <c r="L303" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N303" s="1">
+        <v>30</v>
+      </c>
       <c r="O303" s="1" t="s">
         <v>639</v>
       </c>
@@ -38261,6 +38564,9 @@
       <c r="L304" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N304" s="1">
+        <v>30</v>
+      </c>
       <c r="O304" s="1" t="s">
         <v>639</v>
       </c>
@@ -38338,6 +38644,9 @@
       <c r="L305" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N305" s="1">
+        <v>20</v>
+      </c>
       <c r="O305" s="1" t="s">
         <v>639</v>
       </c>
@@ -38507,6 +38816,9 @@
       <c r="L307" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N307" s="1">
+        <v>60</v>
+      </c>
       <c r="O307" s="1" t="s">
         <v>639</v>
       </c>
@@ -38845,6 +39157,9 @@
       <c r="L311" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N311" s="1">
+        <v>10</v>
+      </c>
       <c r="O311" s="1" t="s">
         <v>639</v>
       </c>
@@ -38931,6 +39246,9 @@
       <c r="L312" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N312" s="1">
+        <v>15</v>
+      </c>
       <c r="O312" s="1" t="s">
         <v>639</v>
       </c>
@@ -39100,6 +39418,9 @@
       <c r="L314" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N314" s="1">
+        <v>25</v>
+      </c>
       <c r="O314" s="1" t="s">
         <v>639</v>
       </c>
@@ -39183,6 +39504,9 @@
       <c r="L315" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N315" s="1">
+        <v>10</v>
+      </c>
       <c r="O315" s="1" t="s">
         <v>639</v>
       </c>
@@ -39266,6 +39590,9 @@
       <c r="L316" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N316" s="1">
+        <v>5</v>
+      </c>
       <c r="O316" s="1" t="s">
         <v>640</v>
       </c>
@@ -39610,6 +39937,9 @@
       <c r="L320" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N320" s="1">
+        <v>30</v>
+      </c>
       <c r="O320" s="1" t="s">
         <v>639</v>
       </c>
@@ -39696,6 +40026,9 @@
       <c r="L321" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N321" s="1">
+        <v>40</v>
+      </c>
       <c r="O321" s="1" t="s">
         <v>639</v>
       </c>
@@ -40224,6 +40557,9 @@
       <c r="L327" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N327" s="1">
+        <v>2</v>
+      </c>
       <c r="O327" s="1" t="s">
         <v>640</v>
       </c>
@@ -40648,6 +40984,9 @@
       <c r="L332" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N332" s="1">
+        <v>20</v>
+      </c>
       <c r="O332" s="1" t="s">
         <v>639</v>
       </c>
@@ -40817,6 +41156,9 @@
       <c r="L334" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N334" s="1">
+        <v>30</v>
+      </c>
       <c r="O334" s="1" t="s">
         <v>639</v>
       </c>
@@ -40986,6 +41328,9 @@
       <c r="L336" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N336" s="1">
+        <v>20</v>
+      </c>
       <c r="O336" s="1" t="s">
         <v>639</v>
       </c>
@@ -41439,6 +41784,9 @@
       <c r="L341" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N341" s="1">
+        <v>6</v>
+      </c>
       <c r="O341" s="1" t="s">
         <v>640</v>
       </c>
@@ -41798,6 +42146,9 @@
       <c r="L345" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N345" s="1">
+        <v>30</v>
+      </c>
       <c r="O345" s="1" t="s">
         <v>639</v>
       </c>
@@ -41878,6 +42229,9 @@
       <c r="L346" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N346" s="1">
+        <v>30</v>
+      </c>
       <c r="O346" s="1" t="s">
         <v>639</v>
       </c>
@@ -42231,6 +42585,12 @@
       <c r="L350" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="M350" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="N350" s="1">
+        <v>7</v>
+      </c>
       <c r="O350" s="1" t="s">
         <v>640</v>
       </c>
@@ -42676,6 +43036,9 @@
       <c r="L355" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N355" s="1">
+        <v>1</v>
+      </c>
       <c r="O355" s="1" t="s">
         <v>640</v>
       </c>
@@ -42942,6 +43305,9 @@
       <c r="L358" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N358" s="1">
+        <v>1</v>
+      </c>
       <c r="O358" s="1" t="s">
         <v>640</v>
       </c>
@@ -43022,6 +43388,9 @@
       <c r="L359" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N359" s="1">
+        <v>1</v>
+      </c>
       <c r="O359" s="1" t="s">
         <v>640</v>
       </c>
@@ -43191,6 +43560,12 @@
       <c r="L361" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="M361" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="N361" s="1">
+        <v>1</v>
+      </c>
       <c r="O361" s="1" t="s">
         <v>640</v>
       </c>
@@ -43277,6 +43652,9 @@
       <c r="L362" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N362" s="1">
+        <v>10</v>
+      </c>
       <c r="O362" s="1" t="s">
         <v>639</v>
       </c>
@@ -43449,6 +43827,9 @@
       <c r="L364" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N364" s="1">
+        <v>1</v>
+      </c>
       <c r="O364" s="1" t="s">
         <v>640</v>
       </c>
@@ -43707,6 +44088,9 @@
       <c r="L367" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N367" s="1">
+        <v>7</v>
+      </c>
       <c r="O367" s="1" t="s">
         <v>640</v>
       </c>
@@ -43790,6 +44174,9 @@
       <c r="L368" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N368" s="1">
+        <v>20</v>
+      </c>
       <c r="O368" s="1" t="s">
         <v>639</v>
       </c>
@@ -43873,6 +44260,9 @@
       <c r="L369" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N369" s="1">
+        <v>1</v>
+      </c>
       <c r="O369" s="1" t="s">
         <v>640</v>
       </c>
@@ -43950,6 +44340,9 @@
       <c r="L370" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N370" s="1">
+        <v>30</v>
+      </c>
       <c r="O370" s="1" t="s">
         <v>639</v>
       </c>
@@ -44211,6 +44604,9 @@
       <c r="L373" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N373" s="1">
+        <v>20</v>
+      </c>
       <c r="O373" s="1" t="s">
         <v>639</v>
       </c>
@@ -44294,6 +44690,9 @@
       <c r="L374" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N374" s="1">
+        <v>40</v>
+      </c>
       <c r="O374" s="1" t="s">
         <v>639</v>
       </c>
@@ -44377,6 +44776,9 @@
       <c r="L375" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N375" s="1">
+        <v>10</v>
+      </c>
       <c r="O375" s="1" t="s">
         <v>639</v>
       </c>
@@ -44460,6 +44862,9 @@
       <c r="L376" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N376" s="1">
+        <v>20</v>
+      </c>
       <c r="O376" s="1" t="s">
         <v>639</v>
       </c>
@@ -44543,6 +44948,9 @@
       <c r="L377" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N377" s="1">
+        <v>10</v>
+      </c>
       <c r="O377" s="1" t="s">
         <v>639</v>
       </c>
@@ -44620,6 +45028,9 @@
       <c r="L378" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N378" s="1">
+        <v>40</v>
+      </c>
       <c r="O378" s="1" t="s">
         <v>639</v>
       </c>
@@ -44691,6 +45102,9 @@
       <c r="L379" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N379" s="1">
+        <v>2</v>
+      </c>
       <c r="O379" s="1" t="s">
         <v>640</v>
       </c>
@@ -45020,6 +45434,9 @@
       <c r="L383" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N383" s="1">
+        <v>1</v>
+      </c>
       <c r="O383" s="1" t="s">
         <v>640</v>
       </c>
@@ -45539,6 +45956,9 @@
       <c r="L389" s="1" t="s">
         <v>693</v>
       </c>
+      <c r="N389" s="1">
+        <v>20</v>
+      </c>
       <c r="O389" s="1" t="s">
         <v>639</v>
       </c>
@@ -45678,9 +46098,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE390" xr:uid="{A5379F05-A2B9-4B77-B06E-FCC7CE830BF0}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AD390">
-    <sortCondition ref="A4"/>
+  <autoFilter ref="A1:AE390" xr:uid="{A5379F05-A2B9-4B77-B06E-FCC7CE830BF0}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:AE389">
+      <sortCondition ref="O1:O390"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AF390">
+    <sortCondition ref="A2:A390"/>
   </sortState>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
change some links as test
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1286" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{0B70F582-7E55-4ACA-AAA1-93FB383C3215}"/>
+  <xr:revisionPtr revIDLastSave="1290" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{6E23D7B2-2D76-46E7-A9DC-944172B3CD5E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2232,9 +2232,6 @@
     <t>associatedMedia</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49870035637 | https://www.flickr.com/photos/188303672@N05/49869195813</t>
-  </si>
-  <si>
     <t>https://www.flickr.com/photos/188303672@N05/49869728111 | https://www.flickr.com/photos/188303672@N05/49869195368 | https://www.flickr.com/photos/188303672@N05/49869195703</t>
   </si>
   <si>
@@ -2307,9 +2304,6 @@
     <t>https://www.flickr.com/photos/188303672@N05/49870170392 | https://www.flickr.com/photos/188303672@N05/49869864536</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49869957666</t>
-  </si>
-  <si>
     <t>https://www.flickr.com/photos/188303672@N05/49870312996</t>
   </si>
   <si>
@@ -2328,18 +2322,6 @@
     <t>https://www.flickr.com/photos/188303672@N05/49870263932 | https://www.flickr.com/photos/188303672@N05/49869811396 | https://www.flickr.com/photos/188303672@N05/49870116992</t>
   </si>
   <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49869955676 | https://www.flickr.com/photos/188303672@N05/49869728111 | https://www.flickr.com/photos/188303672@N05/49869195368 | https://www.flickr.com/photos/188303672@N05/49869195703</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49869955676 | https://www.flickr.com/photos/188303672@N05/49870035637 | https://www.flickr.com/photos/188303672@N05/49869195813</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49869955676 | https://www.flickr.com/photos/188303672@N05/49869727676</t>
-  </si>
-  <si>
-    <t>https://www.flickr.com/photos/188303672@N05/49869955676 | https://www.flickr.com/photos/188303672@N05/49869277488 | https://www.flickr.com/photos/188303672@N05/49870116482 | https://www.flickr.com/photos/188303672@N05/49870116242 | https://www.flickr.com/photos/188303672@N05/49870115992</t>
-  </si>
-  <si>
     <t>https://www.flickr.com/photos/188303672@N05/49869419663</t>
   </si>
   <si>
@@ -2416,6 +2398,24 @@
   </si>
   <si>
     <t>https://www.researchgate.net/publication/339181680 | https://www.flickr.com/photos/188303672@N05/49869277488 | https://www.flickr.com/photos/188303672@N05/49870116482</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49869957666_e5a31f3802_b.jpg</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49870035637_bb85fbdc58_b.jpg | https://live.staticflickr.com/65535/49869195813_d39b8a9c2f_b.jpg</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49869955676_c427762a85_b.jpg | https://www.flickr.com/photos/188303672@N05/49869728111 | https://www.flickr.com/photos/188303672@N05/49869195368 | https://www.flickr.com/photos/188303672@N05/49869195703</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49869955676_c427762a85_b.jpg | https://live.staticflickr.com/65535/49870035637_bb85fbdc58_b.jpg | https://live.staticflickr.com/65535/49869195813_d39b8a9c2f_b.jpg</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49869955676_c427762a85_b.jpg | https://www.flickr.com/photos/188303672@N05/49869277488 | https://www.flickr.com/photos/188303672@N05/49870116482 | https://www.flickr.com/photos/188303672@N05/49870116242 | https://www.flickr.com/photos/188303672@N05/49870115992</t>
+  </si>
+  <si>
+    <t>https://live.staticflickr.com/65535/49869955676_c427762a85_b.jpg | https://www.flickr.com/photos/188303672@N05/49869727676</t>
   </si>
 </sst>
 </file>
@@ -3338,7 +3338,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CEF22A8F-0723-4324-AF1E-E428D124E2EC}" type="CELLRANGE">
+                    <a:fld id="{2469B431-B9D6-4445-9427-4CDF03D0881A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3372,7 +3372,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{62E3F096-D13A-45B2-B5B0-E2196D2F9430}" type="CELLRANGE">
+                    <a:fld id="{770BA30E-E0B7-46F6-ABDA-510231745512}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3406,7 +3406,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B7D5ABCA-E029-43F1-A964-1FF6BDB84E39}" type="CELLRANGE">
+                    <a:fld id="{242328A8-8F26-4DF1-ADE6-DE8D7812AA59}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3440,7 +3440,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{EE64C76C-AED0-42F9-AD5A-2643BBACC889}" type="CELLRANGE">
+                    <a:fld id="{E31DEA24-825E-40A6-B6D6-EE421C6163B6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3474,7 +3474,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D3D92A31-5114-4F43-A769-417FA3000370}" type="CELLRANGE">
+                    <a:fld id="{437402FD-E48C-41F6-8365-90D944193C02}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3508,7 +3508,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{44175968-F17B-4E9A-86C2-92BC20A1F23B}" type="CELLRANGE">
+                    <a:fld id="{5129B5D6-B64A-4FD8-8D80-9F325E333975}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3542,7 +3542,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4884D3FF-1625-4610-BC38-498D8805FE3A}" type="CELLRANGE">
+                    <a:fld id="{307314B0-BD8B-4964-A7AC-E272D82214ED}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3576,7 +3576,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{49B6C4F9-5217-4E93-9FC9-899A9C8B9E57}" type="CELLRANGE">
+                    <a:fld id="{E3B4821A-B45C-4337-96CA-1A4C6A3F4933}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3610,7 +3610,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D825580-3A37-4BB1-8DF6-C81DB82E1C32}" type="CELLRANGE">
+                    <a:fld id="{E74108EF-14BE-46BC-95DF-604E13C69E01}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3644,7 +3644,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6E9BEC5F-DBB1-46E1-9B2E-19A653E32219}" type="CELLRANGE">
+                    <a:fld id="{C4D959D3-43F9-4762-9AD8-8E5606DA393E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3678,7 +3678,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CFE062CE-7E69-4DBE-BA97-F336F7F67E49}" type="CELLRANGE">
+                    <a:fld id="{156A4798-0BB9-4F72-848B-2968B180180E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3712,7 +3712,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8E3E1AFA-E46E-4DBA-8F37-A69020106C97}" type="CELLRANGE">
+                    <a:fld id="{F35D0113-0CFA-4110-A7CE-5DE61BE575B7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3746,7 +3746,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{799BEE7D-ECD5-466B-A39A-A42D074B79C7}" type="CELLRANGE">
+                    <a:fld id="{8C2A7C2F-7B56-4C8A-B1FC-59F415B99B96}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3780,7 +3780,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6CC2E56F-CA75-411A-8A76-5F9CFB18E7C2}" type="CELLRANGE">
+                    <a:fld id="{8FA9E44D-41E7-43B8-B95F-B14AF0015EE1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3814,7 +3814,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA852F27-16A1-4122-BC39-3714A1994F99}" type="CELLRANGE">
+                    <a:fld id="{43FD954C-CCB3-4E7F-B430-7623584D952F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3848,7 +3848,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9A9171F0-5688-4E98-8E66-4DC3AFA63DA9}" type="CELLRANGE">
+                    <a:fld id="{83937602-60C3-4BAC-ABA9-C1DE4693C97A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3882,7 +3882,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0BC42018-1B34-4247-9C2C-6D3C9E9D8F0D}" type="CELLRANGE">
+                    <a:fld id="{2E23CAE0-9E95-46C8-929B-C6B7122B17F8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3916,7 +3916,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5E53EAA9-A4F8-4836-B11C-061C2C9A5870}" type="CELLRANGE">
+                    <a:fld id="{0F5976E9-3F9F-49F6-B5D3-EBE8528B21E7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3950,7 +3950,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{145DB8F7-FEED-4F19-882A-79025E34A6FA}" type="CELLRANGE">
+                    <a:fld id="{57752568-3F53-478E-B0C9-2A7AD7D87BDC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3984,7 +3984,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{08F9E679-1A80-4DEC-A0C0-9B1552827945}" type="CELLRANGE">
+                    <a:fld id="{D94285F3-5E29-4E2C-9A65-AF39DA964109}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4018,7 +4018,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{72FC844F-24EA-4926-93B4-62C788C53998}" type="CELLRANGE">
+                    <a:fld id="{034010A6-365A-47A4-86A5-52E434FC7BA9}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4052,7 +4052,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5C80B533-DF2E-4B1F-8BF2-EE8A102108E1}" type="CELLRANGE">
+                    <a:fld id="{8C8AFEDA-4E30-4324-B67C-BE6937D8031B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4086,7 +4086,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C1E9B256-1C4E-43CB-9B46-C8233D7A85DC}" type="CELLRANGE">
+                    <a:fld id="{1E4ADC90-0E9A-43F0-9E64-59EB49804E35}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4120,7 +4120,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3FE75835-D9F7-44D9-802D-B1D37B7C9EA7}" type="CELLRANGE">
+                    <a:fld id="{A02A7D66-B292-46BB-97C9-726D7D4CFE8C}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4154,7 +4154,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{2D4B0485-0DD8-4EA4-879B-B4E03BA4896C}" type="CELLRANGE">
+                    <a:fld id="{ECDE4807-DFB7-49A1-A520-04B4FC7462A1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4188,7 +4188,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{984E17CD-B8BB-45D7-B46D-D6DEB019DEE0}" type="CELLRANGE">
+                    <a:fld id="{D6E7F3D7-5C29-4218-AD87-5F9142BD3DD8}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4222,7 +4222,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{58D2E972-0B98-4406-942A-E959EBFA55D3}" type="CELLRANGE">
+                    <a:fld id="{978F345E-5343-40A3-8E62-A498E6F92BDB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -13131,8 +13131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG390"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AG2" sqref="AG2:AG1048576"/>
+    <sheetView tabSelected="1" topLeftCell="X2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13360,7 +13360,7 @@
         <v>718</v>
       </c>
       <c r="AG2" t="s">
-        <v>753</v>
+        <v>784</v>
       </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
@@ -13449,7 +13449,7 @@
         <v>716</v>
       </c>
       <c r="AG3" s="1" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
@@ -13529,7 +13529,7 @@
         <v>715</v>
       </c>
       <c r="AG4" s="1" t="s">
-        <v>760</v>
+        <v>786</v>
       </c>
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
@@ -13609,7 +13609,7 @@
         <v>716</v>
       </c>
       <c r="AG5" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
@@ -13692,7 +13692,7 @@
         <v>716</v>
       </c>
       <c r="AG6" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
@@ -13772,7 +13772,7 @@
         <v>715</v>
       </c>
       <c r="AG7" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
@@ -13852,7 +13852,7 @@
         <v>716</v>
       </c>
       <c r="AG8" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
@@ -13945,7 +13945,7 @@
         <v>716</v>
       </c>
       <c r="AG9" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
@@ -14025,7 +14025,7 @@
         <v>715</v>
       </c>
       <c r="AG10" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
@@ -14286,7 +14286,7 @@
         <v>715</v>
       </c>
       <c r="AG13" s="1" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
@@ -15914,7 +15914,7 @@
         <v>715</v>
       </c>
       <c r="AG32" t="s">
-        <v>764</v>
+        <v>758</v>
       </c>
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
@@ -16086,7 +16086,7 @@
         <v>715</v>
       </c>
       <c r="AG34" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.3">
@@ -16516,7 +16516,7 @@
         <v>715</v>
       </c>
       <c r="AG39" s="1" t="s">
-        <v>728</v>
+        <v>785</v>
       </c>
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.3">
@@ -16605,7 +16605,7 @@
         <v>715</v>
       </c>
       <c r="AG40" s="1" t="s">
-        <v>728</v>
+        <v>785</v>
       </c>
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.3">
@@ -16694,7 +16694,7 @@
         <v>715</v>
       </c>
       <c r="AG41" s="1" t="s">
-        <v>761</v>
+        <v>787</v>
       </c>
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.3">
@@ -16783,7 +16783,7 @@
         <v>715</v>
       </c>
       <c r="AG42" s="1" t="s">
-        <v>728</v>
+        <v>785</v>
       </c>
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.3">
@@ -16872,7 +16872,7 @@
         <v>715</v>
       </c>
       <c r="AG43" s="1" t="s">
-        <v>728</v>
+        <v>785</v>
       </c>
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.3">
@@ -17038,7 +17038,7 @@
         <v>715</v>
       </c>
       <c r="AG45" s="1" t="s">
-        <v>760</v>
+        <v>786</v>
       </c>
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.3">
@@ -17118,7 +17118,7 @@
         <v>716</v>
       </c>
       <c r="AG46" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.3">
@@ -17201,7 +17201,7 @@
         <v>716</v>
       </c>
       <c r="AG47" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.3">
@@ -17281,7 +17281,7 @@
         <v>715</v>
       </c>
       <c r="AG48" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.3">
@@ -17361,7 +17361,7 @@
         <v>716</v>
       </c>
       <c r="AG49" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.3">
@@ -17441,7 +17441,7 @@
         <v>715</v>
       </c>
       <c r="AG50" s="1" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.3">
@@ -17527,7 +17527,7 @@
         <v>715</v>
       </c>
       <c r="AG51" s="1" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.3">
@@ -17610,7 +17610,7 @@
         <v>715</v>
       </c>
       <c r="AG52" s="1" t="s">
-        <v>763</v>
+        <v>788</v>
       </c>
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.3">
@@ -17702,7 +17702,7 @@
         <v>715</v>
       </c>
       <c r="AG53" s="1" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.3">
@@ -17788,7 +17788,7 @@
         <v>715</v>
       </c>
       <c r="AG54" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.3">
@@ -17877,7 +17877,7 @@
         <v>715</v>
       </c>
       <c r="AG55" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.3">
@@ -17966,7 +17966,7 @@
         <v>715</v>
       </c>
       <c r="AG56" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.3">
@@ -18055,7 +18055,7 @@
         <v>715</v>
       </c>
       <c r="AG57" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.3">
@@ -18144,7 +18144,7 @@
         <v>715</v>
       </c>
       <c r="AG58" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.3">
@@ -18233,7 +18233,7 @@
         <v>715</v>
       </c>
       <c r="AG59" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.3">
@@ -18322,7 +18322,7 @@
         <v>715</v>
       </c>
       <c r="AG60" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.3">
@@ -18408,7 +18408,7 @@
         <v>715</v>
       </c>
       <c r="AG61" s="1" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.3">
@@ -18497,7 +18497,7 @@
         <v>715</v>
       </c>
       <c r="AG62" s="1" t="s">
-        <v>787</v>
+        <v>781</v>
       </c>
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.3">
@@ -18586,7 +18586,7 @@
         <v>715</v>
       </c>
       <c r="AG63" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.3">
@@ -18675,7 +18675,7 @@
         <v>715</v>
       </c>
       <c r="AG64" s="1" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.3">
@@ -18767,7 +18767,7 @@
         <v>716</v>
       </c>
       <c r="AG65" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.3">
@@ -18859,7 +18859,7 @@
         <v>716</v>
       </c>
       <c r="AG66" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.3">
@@ -18945,7 +18945,7 @@
         <v>716</v>
       </c>
       <c r="AG67" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.3">
@@ -19034,7 +19034,7 @@
         <v>715</v>
       </c>
       <c r="AG68" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.3">
@@ -19120,7 +19120,7 @@
         <v>716</v>
       </c>
       <c r="AG69" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.3">
@@ -19206,7 +19206,7 @@
         <v>716</v>
       </c>
       <c r="AG70" s="1" t="s">
-        <v>768</v>
+        <v>762</v>
       </c>
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.3">
@@ -19292,7 +19292,7 @@
         <v>716</v>
       </c>
       <c r="AG71" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.3">
@@ -19381,7 +19381,7 @@
         <v>716</v>
       </c>
       <c r="AG72" s="1" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.3">
@@ -19467,7 +19467,7 @@
         <v>716</v>
       </c>
       <c r="AG73" s="1" t="s">
-        <v>767</v>
+        <v>761</v>
       </c>
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.3">
@@ -19556,7 +19556,7 @@
         <v>715</v>
       </c>
       <c r="AG74" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.3">
@@ -19648,7 +19648,7 @@
         <v>715</v>
       </c>
       <c r="AG75" s="1" t="s">
-        <v>762</v>
+        <v>789</v>
       </c>
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.3">
@@ -19737,7 +19737,7 @@
         <v>715</v>
       </c>
       <c r="AG76" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.3">
@@ -19823,7 +19823,7 @@
         <v>715</v>
       </c>
       <c r="AG77" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.3">
@@ -19912,7 +19912,7 @@
         <v>715</v>
       </c>
       <c r="AG78" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.3">
@@ -20001,7 +20001,7 @@
         <v>715</v>
       </c>
       <c r="AG79" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.3">
@@ -20090,7 +20090,7 @@
         <v>715</v>
       </c>
       <c r="AG80" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.3">
@@ -20183,7 +20183,7 @@
         <v>715</v>
       </c>
       <c r="AG81" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.3">
@@ -20272,7 +20272,7 @@
         <v>715</v>
       </c>
       <c r="AG82" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.3">
@@ -20361,7 +20361,7 @@
         <v>715</v>
       </c>
       <c r="AG83" s="1" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.3">
@@ -20613,7 +20613,7 @@
         <v>715</v>
       </c>
       <c r="AG86" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.3">
@@ -20693,7 +20693,7 @@
         <v>715</v>
       </c>
       <c r="AG87" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.3">
@@ -20773,7 +20773,7 @@
         <v>715</v>
       </c>
       <c r="AG88" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.3">
@@ -20856,7 +20856,7 @@
         <v>715</v>
       </c>
       <c r="AG89" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.3">
@@ -20936,7 +20936,7 @@
         <v>715</v>
       </c>
       <c r="AG90" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.3">
@@ -21016,7 +21016,7 @@
         <v>715</v>
       </c>
       <c r="AG91" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.3">
@@ -21096,7 +21096,7 @@
         <v>715</v>
       </c>
       <c r="AG92" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.3">
@@ -21176,7 +21176,7 @@
         <v>715</v>
       </c>
       <c r="AG93" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.3">
@@ -21253,7 +21253,7 @@
         <v>715</v>
       </c>
       <c r="AG94" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.3">
@@ -21337,7 +21337,7 @@
         <v>715</v>
       </c>
       <c r="AG95" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.3">
@@ -21420,7 +21420,7 @@
         <v>715</v>
       </c>
       <c r="AG96" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="97" spans="1:33" x14ac:dyDescent="0.3">
@@ -21500,7 +21500,7 @@
         <v>715</v>
       </c>
       <c r="AG97" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="98" spans="1:33" x14ac:dyDescent="0.3">
@@ -21586,7 +21586,7 @@
         <v>715</v>
       </c>
       <c r="AG98" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="99" spans="1:33" x14ac:dyDescent="0.3">
@@ -21663,7 +21663,7 @@
         <v>715</v>
       </c>
       <c r="AG99" s="1" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
     </row>
     <row r="100" spans="1:33" x14ac:dyDescent="0.3">
@@ -22099,7 +22099,7 @@
         <v>717</v>
       </c>
       <c r="AG104" s="1" t="s">
-        <v>771</v>
+        <v>765</v>
       </c>
     </row>
     <row r="105" spans="1:33" x14ac:dyDescent="0.3">
@@ -22185,7 +22185,7 @@
         <v>717</v>
       </c>
       <c r="AG105" s="1" t="s">
-        <v>769</v>
+        <v>763</v>
       </c>
     </row>
     <row r="106" spans="1:33" x14ac:dyDescent="0.3">
@@ -22268,7 +22268,7 @@
         <v>717</v>
       </c>
       <c r="AG106" s="1" t="s">
-        <v>770</v>
+        <v>764</v>
       </c>
     </row>
     <row r="107" spans="1:33" x14ac:dyDescent="0.3">
@@ -22351,7 +22351,7 @@
         <v>717</v>
       </c>
       <c r="AG107" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.3">
@@ -22431,7 +22431,7 @@
         <v>715</v>
       </c>
       <c r="AG108" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="109" spans="1:33" x14ac:dyDescent="0.3">
@@ -22511,7 +22511,7 @@
         <v>715</v>
       </c>
       <c r="AG109" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="110" spans="1:33" x14ac:dyDescent="0.3">
@@ -22591,7 +22591,7 @@
         <v>715</v>
       </c>
       <c r="AG110" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="111" spans="1:33" x14ac:dyDescent="0.3">
@@ -22674,7 +22674,7 @@
         <v>715</v>
       </c>
       <c r="AG111" s="1" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
     </row>
     <row r="112" spans="1:33" x14ac:dyDescent="0.3">
@@ -22754,7 +22754,7 @@
         <v>715</v>
       </c>
       <c r="AG112" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="113" spans="1:33" x14ac:dyDescent="0.3">
@@ -22834,7 +22834,7 @@
         <v>715</v>
       </c>
       <c r="AG113" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="114" spans="1:33" x14ac:dyDescent="0.3">
@@ -22914,7 +22914,7 @@
         <v>715</v>
       </c>
       <c r="AG114" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="115" spans="1:33" x14ac:dyDescent="0.3">
@@ -22994,7 +22994,7 @@
         <v>715</v>
       </c>
       <c r="AG115" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="116" spans="1:33" x14ac:dyDescent="0.3">
@@ -23071,7 +23071,7 @@
         <v>715</v>
       </c>
       <c r="AG116" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="117" spans="1:33" x14ac:dyDescent="0.3">
@@ -23155,7 +23155,7 @@
         <v>715</v>
       </c>
       <c r="AG117" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="118" spans="1:33" x14ac:dyDescent="0.3">
@@ -23238,7 +23238,7 @@
         <v>715</v>
       </c>
       <c r="AG118" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="119" spans="1:33" x14ac:dyDescent="0.3">
@@ -23318,7 +23318,7 @@
         <v>715</v>
       </c>
       <c r="AG119" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="120" spans="1:33" x14ac:dyDescent="0.3">
@@ -23404,7 +23404,7 @@
         <v>715</v>
       </c>
       <c r="AG120" s="1" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
     </row>
     <row r="121" spans="1:33" x14ac:dyDescent="0.3">
@@ -23481,7 +23481,7 @@
         <v>715</v>
       </c>
       <c r="AG121" s="1" t="s">
-        <v>774</v>
+        <v>768</v>
       </c>
     </row>
     <row r="122" spans="1:33" x14ac:dyDescent="0.3">
@@ -24864,7 +24864,7 @@
         <v>715</v>
       </c>
       <c r="AG137" s="1" t="s">
-        <v>775</v>
+        <v>769</v>
       </c>
     </row>
     <row r="138" spans="1:33" x14ac:dyDescent="0.3">
@@ -24953,7 +24953,7 @@
         <v>717</v>
       </c>
       <c r="AG138" s="1" t="s">
-        <v>772</v>
+        <v>766</v>
       </c>
     </row>
     <row r="139" spans="1:33" x14ac:dyDescent="0.3">
@@ -25042,7 +25042,7 @@
         <v>715</v>
       </c>
       <c r="AG139" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="140" spans="1:33" x14ac:dyDescent="0.3">
@@ -25131,7 +25131,7 @@
         <v>715</v>
       </c>
       <c r="AG140" s="1" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
     </row>
     <row r="141" spans="1:33" x14ac:dyDescent="0.3">
@@ -25217,7 +25217,7 @@
         <v>717</v>
       </c>
       <c r="AG141" s="1" t="s">
-        <v>773</v>
+        <v>767</v>
       </c>
     </row>
     <row r="142" spans="1:33" x14ac:dyDescent="0.3">
@@ -25309,7 +25309,7 @@
         <v>715</v>
       </c>
       <c r="AG142" s="1" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
     </row>
     <row r="143" spans="1:33" x14ac:dyDescent="0.3">
@@ -25395,7 +25395,7 @@
         <v>715</v>
       </c>
       <c r="AG143" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="144" spans="1:33" x14ac:dyDescent="0.3">
@@ -25481,7 +25481,7 @@
         <v>715</v>
       </c>
       <c r="AG144" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="145" spans="1:33" x14ac:dyDescent="0.3">
@@ -25570,7 +25570,7 @@
         <v>715</v>
       </c>
       <c r="AG145" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="146" spans="1:33" x14ac:dyDescent="0.3">
@@ -25659,7 +25659,7 @@
         <v>715</v>
       </c>
       <c r="AG146" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="147" spans="1:33" x14ac:dyDescent="0.3">
@@ -25748,7 +25748,7 @@
         <v>715</v>
       </c>
       <c r="AG147" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="148" spans="1:33" x14ac:dyDescent="0.3">
@@ -25834,7 +25834,7 @@
         <v>715</v>
       </c>
       <c r="AG148" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="149" spans="1:33" x14ac:dyDescent="0.3">
@@ -25923,7 +25923,7 @@
         <v>715</v>
       </c>
       <c r="AG149" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="150" spans="1:33" x14ac:dyDescent="0.3">
@@ -26015,7 +26015,7 @@
         <v>715</v>
       </c>
       <c r="AG150" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="151" spans="1:33" x14ac:dyDescent="0.3">
@@ -26107,7 +26107,7 @@
         <v>715</v>
       </c>
       <c r="AG151" s="1" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
     </row>
     <row r="152" spans="1:33" x14ac:dyDescent="0.3">
@@ -26196,7 +26196,7 @@
         <v>715</v>
       </c>
       <c r="AG152" s="1" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
     </row>
     <row r="153" spans="1:33" x14ac:dyDescent="0.3">
@@ -26285,7 +26285,7 @@
         <v>715</v>
       </c>
       <c r="AG153" s="1" t="s">
-        <v>788</v>
+        <v>782</v>
       </c>
     </row>
     <row r="154" spans="1:33" x14ac:dyDescent="0.3">
@@ -26801,7 +26801,7 @@
         <v>715</v>
       </c>
       <c r="AG159" t="s">
-        <v>786</v>
+        <v>780</v>
       </c>
     </row>
     <row r="160" spans="1:33" x14ac:dyDescent="0.3">
@@ -27062,7 +27062,7 @@
         <v>715</v>
       </c>
       <c r="AG162" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="163" spans="1:33" x14ac:dyDescent="0.3">
@@ -27151,7 +27151,7 @@
         <v>715</v>
       </c>
       <c r="AG163" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="164" spans="1:33" x14ac:dyDescent="0.3">
@@ -27237,7 +27237,7 @@
         <v>715</v>
       </c>
       <c r="AG164" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="165" spans="1:33" x14ac:dyDescent="0.3">
@@ -27323,7 +27323,7 @@
         <v>715</v>
       </c>
       <c r="AG165" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="166" spans="1:33" x14ac:dyDescent="0.3">
@@ -27415,7 +27415,7 @@
         <v>715</v>
       </c>
       <c r="AG166" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="167" spans="1:33" x14ac:dyDescent="0.3">
@@ -27504,7 +27504,7 @@
         <v>715</v>
       </c>
       <c r="AG167" s="1" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="168" spans="1:33" x14ac:dyDescent="0.3">
@@ -27593,7 +27593,7 @@
         <v>715</v>
       </c>
       <c r="AG168" s="1" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="169" spans="1:33" x14ac:dyDescent="0.3">
@@ -27682,7 +27682,7 @@
         <v>719</v>
       </c>
       <c r="AG169" s="1" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
     </row>
     <row r="170" spans="1:33" x14ac:dyDescent="0.3">
@@ -27771,7 +27771,7 @@
         <v>720</v>
       </c>
       <c r="AG170" s="1" t="s">
-        <v>789</v>
+        <v>783</v>
       </c>
     </row>
     <row r="171" spans="1:33" x14ac:dyDescent="0.3">
@@ -28121,7 +28121,7 @@
         <v>715</v>
       </c>
       <c r="AG174" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="175" spans="1:33" x14ac:dyDescent="0.3">
@@ -28216,7 +28216,7 @@
         <v>715</v>
       </c>
       <c r="AG175" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="176" spans="1:33" x14ac:dyDescent="0.3">
@@ -28305,7 +28305,7 @@
         <v>715</v>
       </c>
       <c r="AG176" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="177" spans="1:33" x14ac:dyDescent="0.3">
@@ -28400,7 +28400,7 @@
         <v>715</v>
       </c>
       <c r="AG177" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="178" spans="1:33" x14ac:dyDescent="0.3">
@@ -28495,7 +28495,7 @@
         <v>715</v>
       </c>
       <c r="AG178" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="179" spans="1:33" x14ac:dyDescent="0.3">
@@ -28584,7 +28584,7 @@
         <v>715</v>
       </c>
       <c r="AG179" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="180" spans="1:33" x14ac:dyDescent="0.3">
@@ -28673,7 +28673,7 @@
         <v>715</v>
       </c>
       <c r="AG180" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="181" spans="1:33" x14ac:dyDescent="0.3">
@@ -28768,7 +28768,7 @@
         <v>715</v>
       </c>
       <c r="AG181" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="182" spans="1:33" x14ac:dyDescent="0.3">
@@ -28863,7 +28863,7 @@
         <v>715</v>
       </c>
       <c r="AG182" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="183" spans="1:33" x14ac:dyDescent="0.3">
@@ -28958,7 +28958,7 @@
         <v>715</v>
       </c>
       <c r="AG183" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="184" spans="1:33" x14ac:dyDescent="0.3">
@@ -29053,7 +29053,7 @@
         <v>715</v>
       </c>
       <c r="AG184" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="185" spans="1:33" x14ac:dyDescent="0.3">
@@ -29145,7 +29145,7 @@
         <v>715</v>
       </c>
       <c r="AG185" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="186" spans="1:33" x14ac:dyDescent="0.3">
@@ -29240,7 +29240,7 @@
         <v>715</v>
       </c>
       <c r="AG186" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="187" spans="1:33" x14ac:dyDescent="0.3">
@@ -29335,7 +29335,7 @@
         <v>715</v>
       </c>
       <c r="AG187" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="188" spans="1:33" x14ac:dyDescent="0.3">
@@ -29424,7 +29424,7 @@
         <v>715</v>
       </c>
       <c r="AG188" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="189" spans="1:33" x14ac:dyDescent="0.3">
@@ -29516,7 +29516,7 @@
         <v>715</v>
       </c>
       <c r="AG189" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="190" spans="1:33" x14ac:dyDescent="0.3">
@@ -29608,7 +29608,7 @@
         <v>715</v>
       </c>
       <c r="AG190" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="191" spans="1:33" x14ac:dyDescent="0.3">
@@ -29700,7 +29700,7 @@
         <v>715</v>
       </c>
       <c r="AG191" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="192" spans="1:33" x14ac:dyDescent="0.3">
@@ -29792,7 +29792,7 @@
         <v>715</v>
       </c>
       <c r="AG192" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="193" spans="1:33" x14ac:dyDescent="0.3">
@@ -29884,7 +29884,7 @@
         <v>715</v>
       </c>
       <c r="AG193" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="194" spans="1:33" x14ac:dyDescent="0.3">
@@ -29976,7 +29976,7 @@
         <v>715</v>
       </c>
       <c r="AG194" s="1" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
     </row>
     <row r="195" spans="1:33" x14ac:dyDescent="0.3">
@@ -30412,7 +30412,7 @@
         <v>715</v>
       </c>
       <c r="AG199" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="200" spans="1:33" x14ac:dyDescent="0.3">
@@ -30495,7 +30495,7 @@
         <v>715</v>
       </c>
       <c r="AG200" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="201" spans="1:33" x14ac:dyDescent="0.3">
@@ -30581,7 +30581,7 @@
         <v>715</v>
       </c>
       <c r="AG201" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="202" spans="1:33" x14ac:dyDescent="0.3">
@@ -30661,7 +30661,7 @@
         <v>715</v>
       </c>
       <c r="AG202" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="203" spans="1:33" x14ac:dyDescent="0.3">
@@ -30747,7 +30747,7 @@
         <v>715</v>
       </c>
       <c r="AG203" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="204" spans="1:33" x14ac:dyDescent="0.3">
@@ -30833,7 +30833,7 @@
         <v>715</v>
       </c>
       <c r="AG204" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="205" spans="1:33" x14ac:dyDescent="0.3">
@@ -30916,7 +30916,7 @@
         <v>715</v>
       </c>
       <c r="AG205" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="206" spans="1:33" x14ac:dyDescent="0.3">
@@ -31011,7 +31011,7 @@
         <v>715</v>
       </c>
       <c r="AG206" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="207" spans="1:33" x14ac:dyDescent="0.3">
@@ -31106,7 +31106,7 @@
         <v>715</v>
       </c>
       <c r="AG207" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="208" spans="1:33" x14ac:dyDescent="0.3">
@@ -31192,7 +31192,7 @@
         <v>715</v>
       </c>
       <c r="AG208" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="209" spans="1:33" x14ac:dyDescent="0.3">
@@ -31282,7 +31282,7 @@
         <v>715</v>
       </c>
       <c r="AG209" s="1" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
     </row>
     <row r="210" spans="1:33" x14ac:dyDescent="0.3">
@@ -31368,7 +31368,7 @@
         <v>715</v>
       </c>
       <c r="AG210" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="211" spans="1:33" x14ac:dyDescent="0.3">
@@ -31460,7 +31460,7 @@
         <v>715</v>
       </c>
       <c r="AG211" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="212" spans="1:33" x14ac:dyDescent="0.3">
@@ -31552,7 +31552,7 @@
         <v>715</v>
       </c>
       <c r="AG212" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="213" spans="1:33" x14ac:dyDescent="0.3">
@@ -31644,7 +31644,7 @@
         <v>715</v>
       </c>
       <c r="AG213" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="214" spans="1:33" x14ac:dyDescent="0.3">
@@ -31736,7 +31736,7 @@
         <v>715</v>
       </c>
       <c r="AG214" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="215" spans="1:33" x14ac:dyDescent="0.3">
@@ -31825,7 +31825,7 @@
         <v>715</v>
       </c>
       <c r="AG215" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="216" spans="1:33" x14ac:dyDescent="0.3">
@@ -31917,7 +31917,7 @@
         <v>715</v>
       </c>
       <c r="AG216" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="217" spans="1:33" x14ac:dyDescent="0.3">
@@ -32000,7 +32000,7 @@
         <v>717</v>
       </c>
       <c r="AG217" s="1" t="s">
-        <v>776</v>
+        <v>770</v>
       </c>
     </row>
     <row r="218" spans="1:33" x14ac:dyDescent="0.3">
@@ -32083,7 +32083,7 @@
         <v>717</v>
       </c>
       <c r="AG218" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="219" spans="1:33" x14ac:dyDescent="0.3">
@@ -32169,7 +32169,7 @@
         <v>715</v>
       </c>
       <c r="AG219" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="220" spans="1:33" x14ac:dyDescent="0.3">
@@ -32261,7 +32261,7 @@
         <v>715</v>
       </c>
       <c r="AG220" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="221" spans="1:33" x14ac:dyDescent="0.3">
@@ -32353,7 +32353,7 @@
         <v>715</v>
       </c>
       <c r="AG221" s="1" t="s">
-        <v>766</v>
+        <v>760</v>
       </c>
     </row>
     <row r="222" spans="1:33" x14ac:dyDescent="0.3">
@@ -32442,7 +32442,7 @@
         <v>715</v>
       </c>
       <c r="AG222" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="223" spans="1:33" x14ac:dyDescent="0.3">
@@ -32525,7 +32525,7 @@
         <v>715</v>
       </c>
       <c r="AG223" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="224" spans="1:33" x14ac:dyDescent="0.3">
@@ -32614,7 +32614,7 @@
         <v>715</v>
       </c>
       <c r="AG224" s="1" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
     </row>
     <row r="225" spans="1:33" x14ac:dyDescent="0.3">
@@ -32706,7 +32706,7 @@
         <v>715</v>
       </c>
       <c r="AG225" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="226" spans="1:33" x14ac:dyDescent="0.3">
@@ -32786,7 +32786,7 @@
         <v>715</v>
       </c>
       <c r="AG226" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="227" spans="1:33" x14ac:dyDescent="0.3">
@@ -32869,7 +32869,7 @@
         <v>715</v>
       </c>
       <c r="AG227" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="228" spans="1:33" x14ac:dyDescent="0.3">
@@ -32961,7 +32961,7 @@
         <v>715</v>
       </c>
       <c r="AG228" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="229" spans="1:33" x14ac:dyDescent="0.3">
@@ -33053,7 +33053,7 @@
         <v>715</v>
       </c>
       <c r="AG229" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="230" spans="1:33" x14ac:dyDescent="0.3">
@@ -33139,7 +33139,7 @@
         <v>715</v>
       </c>
       <c r="AG230" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="231" spans="1:33" x14ac:dyDescent="0.3">
@@ -33225,7 +33225,7 @@
         <v>715</v>
       </c>
       <c r="AG231" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="232" spans="1:33" x14ac:dyDescent="0.3">
@@ -33305,7 +33305,7 @@
         <v>715</v>
       </c>
       <c r="AG232" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="233" spans="1:33" x14ac:dyDescent="0.3">
@@ -33388,7 +33388,7 @@
         <v>715</v>
       </c>
       <c r="AG233" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="234" spans="1:33" x14ac:dyDescent="0.3">
@@ -33477,7 +33477,7 @@
         <v>715</v>
       </c>
       <c r="AG234" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="235" spans="1:33" x14ac:dyDescent="0.3">
@@ -33569,7 +33569,7 @@
         <v>715</v>
       </c>
       <c r="AG235" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="236" spans="1:33" x14ac:dyDescent="0.3">
@@ -33661,7 +33661,7 @@
         <v>715</v>
       </c>
       <c r="AG236" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="237" spans="1:33" x14ac:dyDescent="0.3">
@@ -33753,7 +33753,7 @@
         <v>715</v>
       </c>
       <c r="AG237" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="238" spans="1:33" x14ac:dyDescent="0.3">
@@ -33845,7 +33845,7 @@
         <v>715</v>
       </c>
       <c r="AG238" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="239" spans="1:33" x14ac:dyDescent="0.3">
@@ -33937,7 +33937,7 @@
         <v>715</v>
       </c>
       <c r="AG239" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="240" spans="1:33" x14ac:dyDescent="0.3">
@@ -34017,7 +34017,7 @@
         <v>715</v>
       </c>
       <c r="AG240" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="241" spans="1:33" x14ac:dyDescent="0.3">
@@ -34100,7 +34100,7 @@
         <v>715</v>
       </c>
       <c r="AG241" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="242" spans="1:33" x14ac:dyDescent="0.3">
@@ -34195,7 +34195,7 @@
         <v>715</v>
       </c>
       <c r="AG242" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="243" spans="1:33" x14ac:dyDescent="0.3">
@@ -34290,7 +34290,7 @@
         <v>715</v>
       </c>
       <c r="AG243" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="244" spans="1:33" x14ac:dyDescent="0.3">
@@ -34370,7 +34370,7 @@
         <v>715</v>
       </c>
       <c r="AG244" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="245" spans="1:33" x14ac:dyDescent="0.3">
@@ -34456,7 +34456,7 @@
         <v>715</v>
       </c>
       <c r="AG245" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="246" spans="1:33" x14ac:dyDescent="0.3">
@@ -34545,7 +34545,7 @@
         <v>715</v>
       </c>
       <c r="AG246" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="247" spans="1:33" x14ac:dyDescent="0.3">
@@ -34640,7 +34640,7 @@
         <v>715</v>
       </c>
       <c r="AG247" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="248" spans="1:33" x14ac:dyDescent="0.3">
@@ -34729,7 +34729,7 @@
         <v>715</v>
       </c>
       <c r="AG248" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="249" spans="1:33" x14ac:dyDescent="0.3">
@@ -34812,7 +34812,7 @@
         <v>715</v>
       </c>
       <c r="AG249" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="250" spans="1:33" x14ac:dyDescent="0.3">
@@ -34895,7 +34895,7 @@
         <v>715</v>
       </c>
       <c r="AG250" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="251" spans="1:33" x14ac:dyDescent="0.3">
@@ -34981,7 +34981,7 @@
         <v>715</v>
       </c>
       <c r="AG251" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="252" spans="1:33" x14ac:dyDescent="0.3">
@@ -35064,7 +35064,7 @@
         <v>715</v>
       </c>
       <c r="AG252" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="253" spans="1:33" x14ac:dyDescent="0.3">
@@ -35144,7 +35144,7 @@
         <v>715</v>
       </c>
       <c r="AG253" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="254" spans="1:33" x14ac:dyDescent="0.3">
@@ -35233,7 +35233,7 @@
         <v>715</v>
       </c>
       <c r="AG254" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="255" spans="1:33" x14ac:dyDescent="0.3">
@@ -35319,7 +35319,7 @@
         <v>715</v>
       </c>
       <c r="AG255" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="256" spans="1:33" x14ac:dyDescent="0.3">
@@ -35408,7 +35408,7 @@
         <v>715</v>
       </c>
       <c r="AG256" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="257" spans="1:33" x14ac:dyDescent="0.3">
@@ -35503,7 +35503,7 @@
         <v>715</v>
       </c>
       <c r="AG257" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="258" spans="1:33" x14ac:dyDescent="0.3">
@@ -35595,7 +35595,7 @@
         <v>715</v>
       </c>
       <c r="AG258" s="1" t="s">
-        <v>777</v>
+        <v>771</v>
       </c>
     </row>
     <row r="259" spans="1:33" x14ac:dyDescent="0.3">
@@ -35678,7 +35678,7 @@
         <v>715</v>
       </c>
       <c r="AG259" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="260" spans="1:33" x14ac:dyDescent="0.3">
@@ -35773,7 +35773,7 @@
         <v>715</v>
       </c>
       <c r="AG260" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="261" spans="1:33" x14ac:dyDescent="0.3">
@@ -35865,7 +35865,7 @@
         <v>715</v>
       </c>
       <c r="AG261" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="262" spans="1:33" x14ac:dyDescent="0.3">
@@ -35948,7 +35948,7 @@
         <v>715</v>
       </c>
       <c r="AG262" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="263" spans="1:33" x14ac:dyDescent="0.3">
@@ -36035,7 +36035,7 @@
         <v>715</v>
       </c>
       <c r="AG263" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="264" spans="1:33" x14ac:dyDescent="0.3">
@@ -36115,7 +36115,7 @@
         <v>715</v>
       </c>
       <c r="AG264" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="265" spans="1:33" x14ac:dyDescent="0.3">
@@ -36199,7 +36199,7 @@
         <v>715</v>
       </c>
       <c r="AG265" s="1" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="266" spans="1:33" x14ac:dyDescent="0.3">
@@ -37350,7 +37350,7 @@
         <v>717</v>
       </c>
       <c r="AG279" t="s">
-        <v>778</v>
+        <v>772</v>
       </c>
     </row>
     <row r="280" spans="1:33" x14ac:dyDescent="0.3">
@@ -38333,7 +38333,7 @@
         <v>715</v>
       </c>
       <c r="AG291" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="292" spans="1:33" x14ac:dyDescent="0.3">
@@ -38419,7 +38419,7 @@
         <v>715</v>
       </c>
       <c r="AG292" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="293" spans="1:33" x14ac:dyDescent="0.3">
@@ -38511,7 +38511,7 @@
         <v>715</v>
       </c>
       <c r="AG293" s="1" t="s">
-        <v>779</v>
+        <v>773</v>
       </c>
     </row>
     <row r="294" spans="1:33" x14ac:dyDescent="0.3">
@@ -38603,7 +38603,7 @@
         <v>715</v>
       </c>
       <c r="AG294" s="1" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
     </row>
     <row r="295" spans="1:33" x14ac:dyDescent="0.3">
@@ -39178,7 +39178,7 @@
         <v>715</v>
       </c>
       <c r="AG301" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="302" spans="1:33" x14ac:dyDescent="0.3">
@@ -39270,7 +39270,7 @@
         <v>715</v>
       </c>
       <c r="AG302" s="1" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
     </row>
     <row r="303" spans="1:33" x14ac:dyDescent="0.3">
@@ -39359,7 +39359,7 @@
         <v>715</v>
       </c>
       <c r="AG303" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="304" spans="1:33" x14ac:dyDescent="0.3">
@@ -39442,7 +39442,7 @@
         <v>717</v>
       </c>
       <c r="AG304" s="1" t="s">
-        <v>780</v>
+        <v>774</v>
       </c>
     </row>
     <row r="305" spans="1:33" x14ac:dyDescent="0.3">
@@ -39534,7 +39534,7 @@
         <v>715</v>
       </c>
       <c r="AG305" s="1" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
     <row r="306" spans="1:33" x14ac:dyDescent="0.3">
@@ -39620,7 +39620,7 @@
         <v>715</v>
       </c>
       <c r="AG306" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="307" spans="1:33" x14ac:dyDescent="0.3">
@@ -39709,7 +39709,7 @@
         <v>721</v>
       </c>
       <c r="AG307" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="308" spans="1:33" x14ac:dyDescent="0.3">
@@ -39801,7 +39801,7 @@
         <v>715</v>
       </c>
       <c r="AG308" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="309" spans="1:33" x14ac:dyDescent="0.3">
@@ -39893,7 +39893,7 @@
         <v>715</v>
       </c>
       <c r="AG309" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="310" spans="1:33" x14ac:dyDescent="0.3">
@@ -39979,7 +39979,7 @@
         <v>717</v>
       </c>
       <c r="AG310" s="1" t="s">
-        <v>781</v>
+        <v>775</v>
       </c>
     </row>
     <row r="311" spans="1:33" x14ac:dyDescent="0.3">
@@ -40059,7 +40059,7 @@
         <v>715</v>
       </c>
       <c r="AG311" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="312" spans="1:33" x14ac:dyDescent="0.3">
@@ -40157,7 +40157,7 @@
         <v>715</v>
       </c>
       <c r="AG312" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="313" spans="1:33" x14ac:dyDescent="0.3">
@@ -40243,7 +40243,7 @@
         <v>715</v>
       </c>
       <c r="AG313" s="1" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
     </row>
     <row r="314" spans="1:33" x14ac:dyDescent="0.3">
@@ -40332,7 +40332,7 @@
         <v>716</v>
       </c>
       <c r="AG314" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="315" spans="1:33" x14ac:dyDescent="0.3">
@@ -40421,7 +40421,7 @@
         <v>716</v>
       </c>
       <c r="AG315" s="1" t="s">
-        <v>782</v>
+        <v>776</v>
       </c>
     </row>
     <row r="316" spans="1:33" x14ac:dyDescent="0.3">
@@ -40504,7 +40504,7 @@
         <v>716</v>
       </c>
       <c r="AG316" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="317" spans="1:33" x14ac:dyDescent="0.3">
@@ -40596,7 +40596,7 @@
         <v>722</v>
       </c>
       <c r="AG317" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="318" spans="1:33" x14ac:dyDescent="0.3">
@@ -40688,7 +40688,7 @@
         <v>715</v>
       </c>
       <c r="AG318" s="1" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
     </row>
     <row r="319" spans="1:33" x14ac:dyDescent="0.3">
@@ -40780,7 +40780,7 @@
         <v>716</v>
       </c>
       <c r="AG319" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="320" spans="1:33" x14ac:dyDescent="0.3">
@@ -40872,7 +40872,7 @@
         <v>716</v>
       </c>
       <c r="AG320" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="321" spans="1:33" x14ac:dyDescent="0.3">
@@ -40961,7 +40961,7 @@
         <v>716</v>
       </c>
       <c r="AG321" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="322" spans="1:33" x14ac:dyDescent="0.3">
@@ -41053,7 +41053,7 @@
         <v>716</v>
       </c>
       <c r="AG322" s="1" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
     </row>
     <row r="323" spans="1:33" x14ac:dyDescent="0.3">
@@ -41145,7 +41145,7 @@
         <v>716</v>
       </c>
       <c r="AG323" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="324" spans="1:33" x14ac:dyDescent="0.3">
@@ -41237,7 +41237,7 @@
         <v>716</v>
       </c>
       <c r="AG324" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="325" spans="1:33" x14ac:dyDescent="0.3">
@@ -41329,7 +41329,7 @@
         <v>716</v>
       </c>
       <c r="AG325" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="326" spans="1:33" x14ac:dyDescent="0.3">
@@ -41421,7 +41421,7 @@
         <v>716</v>
       </c>
       <c r="AG326" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="327" spans="1:33" x14ac:dyDescent="0.3">
@@ -41510,7 +41510,7 @@
         <v>716</v>
       </c>
       <c r="AG327" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="328" spans="1:33" x14ac:dyDescent="0.3">
@@ -41602,7 +41602,7 @@
         <v>716</v>
       </c>
       <c r="AG328" s="1" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
     </row>
     <row r="329" spans="1:33" x14ac:dyDescent="0.3">
@@ -41857,7 +41857,7 @@
         <v>717</v>
       </c>
       <c r="AG331" s="1" t="s">
-        <v>783</v>
+        <v>777</v>
       </c>
     </row>
     <row r="332" spans="1:33" x14ac:dyDescent="0.3">
@@ -43111,7 +43111,7 @@
         <v>715</v>
       </c>
       <c r="AG345" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="346" spans="1:33" x14ac:dyDescent="0.3">
@@ -43197,7 +43197,7 @@
         <v>715</v>
       </c>
       <c r="AG346" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="347" spans="1:33" x14ac:dyDescent="0.3">
@@ -43289,7 +43289,7 @@
         <v>715</v>
       </c>
       <c r="AG347" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="348" spans="1:33" x14ac:dyDescent="0.3">
@@ -43381,7 +43381,7 @@
         <v>715</v>
       </c>
       <c r="AG348" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="349" spans="1:33" x14ac:dyDescent="0.3">
@@ -43473,7 +43473,7 @@
         <v>715</v>
       </c>
       <c r="AG349" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="350" spans="1:33" x14ac:dyDescent="0.3">
@@ -43565,7 +43565,7 @@
         <v>715</v>
       </c>
       <c r="AG350" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="351" spans="1:33" x14ac:dyDescent="0.3">
@@ -43657,7 +43657,7 @@
         <v>715</v>
       </c>
       <c r="AG351" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="352" spans="1:33" x14ac:dyDescent="0.3">
@@ -43749,7 +43749,7 @@
         <v>715</v>
       </c>
       <c r="AG352" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="353" spans="1:33" x14ac:dyDescent="0.3">
@@ -43844,7 +43844,7 @@
         <v>715</v>
       </c>
       <c r="AG353" s="1" t="s">
-        <v>784</v>
+        <v>778</v>
       </c>
     </row>
     <row r="354" spans="1:33" x14ac:dyDescent="0.3">
@@ -43939,7 +43939,7 @@
         <v>715</v>
       </c>
       <c r="AG354" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="355" spans="1:33" x14ac:dyDescent="0.3">
@@ -44031,7 +44031,7 @@
         <v>715</v>
       </c>
       <c r="AG355" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="356" spans="1:33" x14ac:dyDescent="0.3">
@@ -44127,7 +44127,7 @@
         <v>715</v>
       </c>
       <c r="AG356" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="357" spans="1:33" x14ac:dyDescent="0.3">
@@ -44223,7 +44223,7 @@
         <v>715</v>
       </c>
       <c r="AG357" s="1" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
     </row>
     <row r="358" spans="1:33" x14ac:dyDescent="0.3">
@@ -44303,7 +44303,7 @@
         <v>715</v>
       </c>
       <c r="AG358" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="359" spans="1:33" x14ac:dyDescent="0.3">
@@ -44386,7 +44386,7 @@
         <v>715</v>
       </c>
       <c r="AG359" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="360" spans="1:33" x14ac:dyDescent="0.3">
@@ -44481,7 +44481,7 @@
         <v>715</v>
       </c>
       <c r="AG360" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="361" spans="1:33" x14ac:dyDescent="0.3">
@@ -44573,7 +44573,7 @@
         <v>715</v>
       </c>
       <c r="AG361" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="362" spans="1:33" x14ac:dyDescent="0.3">
@@ -44668,7 +44668,7 @@
         <v>715</v>
       </c>
       <c r="AG362" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="363" spans="1:33" x14ac:dyDescent="0.3">
@@ -44763,7 +44763,7 @@
         <v>715</v>
       </c>
       <c r="AG363" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="364" spans="1:33" x14ac:dyDescent="0.3">
@@ -44843,7 +44843,7 @@
         <v>717</v>
       </c>
       <c r="AG364" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="365" spans="1:33" x14ac:dyDescent="0.3">
@@ -44935,7 +44935,7 @@
         <v>715</v>
       </c>
       <c r="AG365" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="366" spans="1:33" x14ac:dyDescent="0.3">
@@ -45027,7 +45027,7 @@
         <v>715</v>
       </c>
       <c r="AG366" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="367" spans="1:33" x14ac:dyDescent="0.3">
@@ -45116,7 +45116,7 @@
         <v>715</v>
       </c>
       <c r="AG367" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="368" spans="1:33" x14ac:dyDescent="0.3">
@@ -45205,7 +45205,7 @@
         <v>715</v>
       </c>
       <c r="AG368" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="369" spans="1:33" x14ac:dyDescent="0.3">
@@ -45288,7 +45288,7 @@
         <v>717</v>
       </c>
       <c r="AG369" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="370" spans="1:33" x14ac:dyDescent="0.3">
@@ -45377,7 +45377,7 @@
         <v>715</v>
       </c>
       <c r="AG370" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="371" spans="1:33" x14ac:dyDescent="0.3">
@@ -45469,7 +45469,7 @@
         <v>715</v>
       </c>
       <c r="AG371" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="372" spans="1:33" x14ac:dyDescent="0.3">
@@ -45561,7 +45561,7 @@
         <v>715</v>
       </c>
       <c r="AG372" s="1" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
     </row>
     <row r="373" spans="1:33" x14ac:dyDescent="0.3">
@@ -45650,7 +45650,7 @@
         <v>715</v>
       </c>
       <c r="AG373" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="374" spans="1:33" x14ac:dyDescent="0.3">
@@ -45739,7 +45739,7 @@
         <v>715</v>
       </c>
       <c r="AG374" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="375" spans="1:33" x14ac:dyDescent="0.3">
@@ -45828,7 +45828,7 @@
         <v>715</v>
       </c>
       <c r="AG375" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="376" spans="1:33" x14ac:dyDescent="0.3">
@@ -45917,7 +45917,7 @@
         <v>715</v>
       </c>
       <c r="AG376" s="1" t="s">
-        <v>765</v>
+        <v>759</v>
       </c>
     </row>
     <row r="377" spans="1:33" x14ac:dyDescent="0.3">
@@ -46000,7 +46000,7 @@
         <v>717</v>
       </c>
       <c r="AG377" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="378" spans="1:33" x14ac:dyDescent="0.3">
@@ -46083,7 +46083,7 @@
         <v>717</v>
       </c>
       <c r="AG378" s="1" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
     </row>
     <row r="379" spans="1:33" x14ac:dyDescent="0.3">
@@ -46163,7 +46163,7 @@
         <v>715</v>
       </c>
       <c r="AG379" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="380" spans="1:33" x14ac:dyDescent="0.3">
@@ -46246,7 +46246,7 @@
         <v>715</v>
       </c>
       <c r="AG380" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="381" spans="1:33" x14ac:dyDescent="0.3">
@@ -46329,7 +46329,7 @@
         <v>715</v>
       </c>
       <c r="AG381" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="382" spans="1:33" x14ac:dyDescent="0.3">
@@ -46421,7 +46421,7 @@
         <v>715</v>
       </c>
       <c r="AG382" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="383" spans="1:33" x14ac:dyDescent="0.3">
@@ -46507,7 +46507,7 @@
         <v>715</v>
       </c>
       <c r="AG383" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="384" spans="1:33" x14ac:dyDescent="0.3">
@@ -46593,7 +46593,7 @@
         <v>715</v>
       </c>
       <c r="AG384" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
     </row>
     <row r="385" spans="1:33" x14ac:dyDescent="0.3">
@@ -46685,7 +46685,7 @@
         <v>715</v>
       </c>
       <c r="AG385" s="1" t="s">
-        <v>785</v>
+        <v>779</v>
       </c>
     </row>
     <row r="386" spans="1:33" x14ac:dyDescent="0.3">
@@ -46777,7 +46777,7 @@
         <v>715</v>
       </c>
       <c r="AG386" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="387" spans="1:33" x14ac:dyDescent="0.3">
@@ -46869,7 +46869,7 @@
         <v>715</v>
       </c>
       <c r="AG387" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="388" spans="1:33" x14ac:dyDescent="0.3">
@@ -46961,7 +46961,7 @@
         <v>715</v>
       </c>
       <c r="AG388" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="389" spans="1:33" x14ac:dyDescent="0.3">
@@ -47044,7 +47044,7 @@
         <v>715</v>
       </c>
       <c r="AG389" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
     <row r="390" spans="1:33" x14ac:dyDescent="0.3">
@@ -47139,7 +47139,7 @@
         <v>715</v>
       </c>
       <c r="AG390" s="1" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
species abundance curve final
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1469" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{046913F3-6DBF-47B4-8F78-1A9120595D09}"/>
+  <xr:revisionPtr revIDLastSave="1490" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86923AF8-88F6-481E-9EF6-2FB48909B3A5}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,19 @@
     <sheet name="spec per gen" sheetId="11" r:id="rId5"/>
     <sheet name="taxa_abundance" sheetId="13" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">genus!$D$2:$E$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AG$390</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId7"/>
-    <pivotCache cacheId="3" r:id="rId8"/>
-    <pivotCache cacheId="21" r:id="rId9"/>
-    <pivotCache cacheId="24" r:id="rId10"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -48,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8673" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8673" uniqueCount="803">
   <si>
     <t>orderNumber</t>
   </si>
@@ -2448,6 +2451,15 @@
   </si>
   <si>
     <t>rel. log(observations)</t>
+  </si>
+  <si>
+    <t>Napaeus cf. venegueraenis samen met N. venegueraensis</t>
+  </si>
+  <si>
+    <t>Hemicycla spec. schrappen</t>
+  </si>
+  <si>
+    <t>Hemicycla psathyra cf. temperata samen met Hemicycla psathyra temperata</t>
   </si>
 </sst>
 </file>
@@ -3370,7 +3382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8B7785C9-76F0-49FF-978F-DE030DCBD39F}" type="CELLRANGE">
+                    <a:fld id="{25B91953-E372-43CC-AB90-FC353682EE4E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3404,7 +3416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9FA7672C-BEBA-41D7-A342-1B6D34AAB0F2}" type="CELLRANGE">
+                    <a:fld id="{E41F9129-A823-4AE6-9228-BC780F67B094}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3438,7 +3450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{46AD421D-F0C9-4740-82E9-F743C6FF205A}" type="CELLRANGE">
+                    <a:fld id="{C0A8722F-610C-4285-92E9-F56F498F06FB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3472,7 +3484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F8832F59-4678-473B-83C3-6707AE9DF8CE}" type="CELLRANGE">
+                    <a:fld id="{CC4876FC-ABCB-4B0E-B7BF-4A8460DBDF12}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3506,7 +3518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5F705CC7-95E0-4C31-9E9A-8D00AAD1F633}" type="CELLRANGE">
+                    <a:fld id="{71F3D7F4-68C5-48BE-95B2-7301A392C45A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3540,7 +3552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D7859E6E-9FDF-488F-8276-60FA83067052}" type="CELLRANGE">
+                    <a:fld id="{340B1BD6-B59E-4026-AE1F-FA47AEDADB2A}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3574,7 +3586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9FCBD21-8709-4391-BD98-8F1F6E5E9153}" type="CELLRANGE">
+                    <a:fld id="{94F21806-E123-4F29-AE87-205DAA8080BB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3608,7 +3620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C47C592A-4A99-4A11-A4D1-BDFF80BF6F07}" type="CELLRANGE">
+                    <a:fld id="{AFA593F8-6B10-4C8F-A2D6-156DB5557C10}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3642,7 +3654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{FD885B1D-47E6-4B6B-BDD1-74B7A0AEE8FE}" type="CELLRANGE">
+                    <a:fld id="{7014CC1B-8843-48FE-9EE9-BF399E85B890}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3676,7 +3688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F0B0415C-9E3F-4216-9EFC-774B06AE2E6E}" type="CELLRANGE">
+                    <a:fld id="{BFDCD56A-F8C2-4F28-8D45-54E492046558}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3710,7 +3722,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{8292FC57-258D-4188-ABB4-07E28449BCC3}" type="CELLRANGE">
+                    <a:fld id="{DDA29EE2-6602-4008-99C8-82020063E827}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3744,7 +3756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C9200F9-8DB7-454E-9A96-DCFF7735FC52}" type="CELLRANGE">
+                    <a:fld id="{0812A2CE-20D4-435F-A02B-BF6C0CCD6A33}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3778,7 +3790,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{98D01BC3-71E2-452D-8FB9-E05DE3AF587C}" type="CELLRANGE">
+                    <a:fld id="{CB234CE2-9783-4970-A6C5-D467FBF21B94}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3812,7 +3824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{31C2ACFA-BF00-4E82-A4C4-E515965C2F84}" type="CELLRANGE">
+                    <a:fld id="{C4F4F44B-FD03-4172-8A83-8F62B39ED0A3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3846,7 +3858,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AA4FF574-C861-462F-961A-5CE8888B90D7}" type="CELLRANGE">
+                    <a:fld id="{4A56BC14-A834-40F4-9345-4645D8A87CD6}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3880,7 +3892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F9503955-F732-46F9-9E85-9758CC76F7ED}" type="CELLRANGE">
+                    <a:fld id="{A0E2E6C5-11CB-41FC-8B6D-BCBA91B875FB}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3914,7 +3926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6C2827BB-C50F-4312-A6F5-F9F79F067AB7}" type="CELLRANGE">
+                    <a:fld id="{B1D9611D-8318-40D6-A8BD-343F584A0DF7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3948,7 +3960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0023DA32-478D-4EF0-B163-81893FE78D51}" type="CELLRANGE">
+                    <a:fld id="{9C3F4A9B-56E4-4066-B15D-F2B829EE7E11}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3982,7 +3994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{06A0FD46-1C98-4118-8FCF-C72C3E652697}" type="CELLRANGE">
+                    <a:fld id="{5BA7F935-40E1-4837-9467-66FF352EBC5D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4016,7 +4028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DCDD07B6-26E7-41FB-8338-C062916A185C}" type="CELLRANGE">
+                    <a:fld id="{A7C4C672-2C5F-4546-A98D-A77F6BD9F09F}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4050,7 +4062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B5CE75A5-C1EB-4042-969C-9F3DC2A1D439}" type="CELLRANGE">
+                    <a:fld id="{837DBB51-7AC6-44CF-B520-7D4E5F1B2D62}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4084,7 +4096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5A0DE6D4-E8A4-4999-A177-DEAE0F32990B}" type="CELLRANGE">
+                    <a:fld id="{F460A83D-1D79-44DA-8F78-20BDF3A7BB86}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4118,7 +4130,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{61D55257-9B15-4759-801D-709DDC90D78C}" type="CELLRANGE">
+                    <a:fld id="{30A842FD-8A4C-4DAD-82A1-F319501F70BD}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4152,7 +4164,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7503545B-02DB-42D4-9051-9C44A6DCD532}" type="CELLRANGE">
+                    <a:fld id="{64D6E44F-6AA7-460B-A00F-A0767A8819E7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4186,7 +4198,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{3D9DD763-59E7-4F75-B689-1C5182924659}" type="CELLRANGE">
+                    <a:fld id="{9894C4A2-9D04-4667-BB6F-8468DCCDD13D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4220,7 +4232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B604595C-AD62-4D07-A862-00090650B7D8}" type="CELLRANGE">
+                    <a:fld id="{C18E3EF6-3B35-4D71-A2AC-CDC491D0AAC3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4254,7 +4266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{6723617C-3F46-488A-B063-E8F9AECD1E4D}" type="CELLRANGE">
+                    <a:fld id="{686F1EF0-DB0D-43A0-9C42-E4180A2675E7}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -5317,10 +5329,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>taxa_abundance!$F$3:$F$64</c:f>
+              <c:f>taxa_abundance!$F$3:$F$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5498,24 +5510,15 @@
                 <c:pt idx="58">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>62</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>taxa_abundance!$G$3:$G$64</c:f>
+              <c:f>taxa_abundance!$G$3:$G$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -5538,28 +5541,28 @@
                   <c:v>0.35897435897435898</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.25641025641025639</c:v>
+                  <c:v>0.30769230769230771</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.25641025641025639</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.23076923076923078</c:v>
+                  <c:v>0.25641025641025639</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.23076923076923078</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.20512820512820512</c:v>
+                  <c:v>0.23076923076923078</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.20512820512820512</c:v>
+                  <c:v>0.23076923076923078</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.20512820512820512</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.17948717948717949</c:v>
+                  <c:v>0.20512820512820512</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.17948717948717949</c:v>
@@ -5589,7 +5592,7 @@
                   <c:v>0.12820512820512819</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.12820512820512819</c:v>
+                  <c:v>0.10256410256410256</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0.10256410256410256</c:v>
@@ -5607,7 +5610,7 @@
                   <c:v>0.10256410256410256</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.10256410256410256</c:v>
+                  <c:v>7.6923076923076927E-2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>7.6923076923076927E-2</c:v>
@@ -5631,7 +5634,7 @@
                   <c:v>7.6923076923076927E-2</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.6923076923076927E-2</c:v>
+                  <c:v>5.128205128205128E-2</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>5.128205128205128E-2</c:v>
@@ -5667,7 +5670,7 @@
                   <c:v>5.128205128205128E-2</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>5.128205128205128E-2</c:v>
+                  <c:v>2.564102564102564E-2</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>2.564102564102564E-2</c:v>
@@ -5691,15 +5694,6 @@
                   <c:v>2.564102564102564E-2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.564102564102564E-2</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>2.564102564102564E-2</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>2.564102564102564E-2</c:v>
-                </c:pt>
-                <c:pt idx="61">
                   <c:v>2.564102564102564E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -5727,7 +5721,7 @@
         <c:axId val="481795472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="65"/>
+          <c:max val="60"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -6005,10 +5999,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>taxa_abundance!$F$3:$F$64</c:f>
+              <c:f>taxa_abundance!$F$3:$F$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6186,24 +6180,15 @@
                 <c:pt idx="58">
                   <c:v>59</c:v>
                 </c:pt>
-                <c:pt idx="59">
-                  <c:v>60</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>62</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>taxa_abundance!$I$3:$I$64</c:f>
+              <c:f>taxa_abundance!$I$3:$I$61</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="62"/>
+                <c:ptCount val="59"/>
                 <c:pt idx="0">
                   <c:v>1</c:v>
                 </c:pt>
@@ -6226,28 +6211,28 @@
                   <c:v>0.72035292006162344</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.62850998984188011</c:v>
+                  <c:v>0.6782761939909403</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.62850998984188011</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.59975094991440026</c:v>
+                  <c:v>0.62850998984188011</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>0.59975094991440026</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.56760107855061015</c:v>
+                  <c:v>0.59975094991440026</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.56760107855061015</c:v>
+                  <c:v>0.59975094991440026</c:v>
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.56760107855061015</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.53115256054475335</c:v>
+                  <c:v>0.56760107855061015</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>0.53115256054475335</c:v>
@@ -6277,7 +6262,7 @@
                   <c:v>0.43930963032501014</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.43930963032501014</c:v>
+                  <c:v>0.37840071903374012</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>0.37840071903374012</c:v>
@@ -6295,7 +6280,7 @@
                   <c:v>0.37840071903374012</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.37840071903374012</c:v>
+                  <c:v>0.29987547495720013</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>0.29987547495720013</c:v>
@@ -6319,7 +6304,7 @@
                   <c:v>0.29987547495720013</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.29987547495720013</c:v>
+                  <c:v>0.18920035951687006</c:v>
                 </c:pt>
                 <c:pt idx="39">
                   <c:v>0.18920035951687006</c:v>
@@ -6355,7 +6340,7 @@
                   <c:v>0.18920035951687006</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.18920035951687006</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>0</c:v>
@@ -6379,15 +6364,6 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="61">
                   <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
@@ -6415,7 +6391,7 @@
         <c:axId val="481801376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="65"/>
+          <c:max val="60"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -8954,6 +8930,19 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Sheet7"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="WARD" refreshedDate="43891.590313078705" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="390" xr:uid="{869674DF-0315-4FAD-B166-8FA90FD916D1}">
   <cacheSource type="worksheet">
@@ -25478,7 +25467,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8F3382-6770-4C1E-A264-992B6F7166B5}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{9C8F3382-6770-4C1E-A264-992B6F7166B5}" name="PivotTable1" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -25591,7 +25580,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07D6A4A6-309D-457A-82A4-D13AE5CB1A00}" name="PivotTable14" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{07D6A4A6-309D-457A-82A4-D13AE5CB1A00}" name="PivotTable14" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B32" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -25763,7 +25752,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12E8988F-0A56-4B5E-B133-47C90ED1AD34}" name="PivotTable2" cacheId="21" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{12E8988F-0A56-4B5E-B133-47C90ED1AD34}" name="PivotTable2" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="D7:E35" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField showAll="0"/>
@@ -25908,7 +25897,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C84FBE34-F750-4F2E-AF23-E8F6D1C83A74}" name="PivotTable4" cacheId="24" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{C84FBE34-F750-4F2E-AF23-E8F6D1C83A74}" name="PivotTable4" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B66" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="33">
     <pivotField showAll="0"/>
@@ -26488,7 +26477,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG390"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
@@ -63816,10 +63805,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29377B9E-EE4F-45EE-ABD5-75334AF19FBC}">
-  <dimension ref="A2:I66"/>
+  <dimension ref="A2:M66"/>
   <sheetViews>
-    <sheetView topLeftCell="D7" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -63901,11 +63890,11 @@
         <v>0.97435897435897434</v>
       </c>
       <c r="H4">
-        <f t="shared" ref="H4:H64" si="0">LOG10(E4)</f>
+        <f>LOG10(E4)</f>
         <v>1.5797835966168101</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I64" si="1">H4/$H$3</f>
+        <f>H4/$H$3</f>
         <v>0.99290977226200028</v>
       </c>
     </row>
@@ -63930,11 +63919,11 @@
         <v>0.76923076923076927</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f>LOG10(E5)</f>
         <v>1.4771212547196624</v>
       </c>
       <c r="I5">
-        <f t="shared" si="1"/>
+        <f>H5/$H$3</f>
         <v>0.92838546479908024</v>
       </c>
     </row>
@@ -63959,11 +63948,11 @@
         <v>0.53846153846153844</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f>LOG10(E6)</f>
         <v>1.3222192947339193</v>
       </c>
       <c r="I6">
-        <f t="shared" si="1"/>
+        <f>H6/$H$3</f>
         <v>0.83102803550195359</v>
       </c>
     </row>
@@ -63984,15 +63973,15 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <f t="shared" ref="G5:G64" si="2">E7/$E$3</f>
+        <f>E7/$E$3</f>
         <v>0.51282051282051277</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f>LOG10(E7)</f>
         <v>1.3010299956639813</v>
       </c>
       <c r="I7">
-        <f t="shared" si="1"/>
+        <f>H7/$H$3</f>
         <v>0.8177103493587502</v>
       </c>
     </row>
@@ -64013,15 +64002,15 @@
         <v>6</v>
       </c>
       <c r="G8">
-        <f t="shared" si="2"/>
+        <f>E8/$E$3</f>
         <v>0.4358974358974359</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f>LOG10(E8)</f>
         <v>1.2304489213782739</v>
       </c>
       <c r="I8">
-        <f t="shared" si="1"/>
+        <f>H8/$H$3</f>
         <v>0.77334943907641129</v>
       </c>
     </row>
@@ -64042,15 +64031,15 @@
         <v>7</v>
       </c>
       <c r="G9">
-        <f t="shared" si="2"/>
+        <f>E9/$E$3</f>
         <v>0.35897435897435898</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f>LOG10(E9)</f>
         <v>1.146128035678238</v>
       </c>
       <c r="I9">
-        <f t="shared" si="1"/>
+        <f>H9/$H$3</f>
         <v>0.72035292006162344</v>
       </c>
     </row>
@@ -64062,25 +64051,25 @@
         <v>3</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>222</v>
+        <v>256</v>
       </c>
       <c r="E10" s="8">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="F10">
         <v>8</v>
       </c>
       <c r="G10">
-        <f t="shared" si="2"/>
-        <v>0.25641025641025639</v>
+        <f>E10/$E$3</f>
+        <v>0.30769230769230771</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
-        <v>1</v>
+        <f>LOG10(E10)</f>
+        <v>1.0791812460476249</v>
       </c>
       <c r="I10">
-        <f t="shared" si="1"/>
-        <v>0.62850998984188011</v>
+        <f>H10/$H$3</f>
+        <v>0.6782761939909403</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
@@ -64091,7 +64080,7 @@
         <v>5</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>113</v>
+        <v>222</v>
       </c>
       <c r="E11" s="8">
         <v>10</v>
@@ -64100,15 +64089,15 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <f t="shared" si="2"/>
+        <f>E11/$E$3</f>
         <v>0.25641025641025639</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f>LOG10(E11)</f>
         <v>1</v>
       </c>
       <c r="I11">
-        <f t="shared" si="1"/>
+        <f>H11/$H$3</f>
         <v>0.62850998984188011</v>
       </c>
     </row>
@@ -64120,25 +64109,25 @@
         <v>6</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>232</v>
+        <v>113</v>
       </c>
       <c r="E12" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <v>10</v>
       </c>
       <c r="G12">
-        <f t="shared" si="2"/>
-        <v>0.23076923076923078</v>
+        <f>E12/$E$3</f>
+        <v>0.25641025641025639</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
-        <v>0.95424250943932487</v>
+        <f>LOG10(E12)</f>
+        <v>1</v>
       </c>
       <c r="I12">
-        <f t="shared" si="1"/>
-        <v>0.59975094991440026</v>
+        <f>H12/$H$3</f>
+        <v>0.62850998984188011</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -64149,7 +64138,7 @@
         <v>1</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>170</v>
+        <v>232</v>
       </c>
       <c r="E13" s="8">
         <v>9</v>
@@ -64158,15 +64147,15 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <f t="shared" si="2"/>
+        <f>E13/$E$3</f>
         <v>0.23076923076923078</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f>LOG10(E13)</f>
         <v>0.95424250943932487</v>
       </c>
       <c r="I13">
-        <f t="shared" si="1"/>
+        <f>H13/$H$3</f>
         <v>0.59975094991440026</v>
       </c>
     </row>
@@ -64181,22 +64170,22 @@
         <v>196</v>
       </c>
       <c r="E14" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F14">
         <v>12</v>
       </c>
       <c r="G14">
-        <f t="shared" si="2"/>
-        <v>0.20512820512820512</v>
+        <f>E14/$E$3</f>
+        <v>0.23076923076923078</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
-        <v>0.90308998699194354</v>
+        <f>LOG10(E14)</f>
+        <v>0.95424250943932487</v>
       </c>
       <c r="I14">
-        <f t="shared" si="1"/>
-        <v>0.56760107855061015</v>
+        <f>H14/$H$3</f>
+        <v>0.59975094991440026</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
@@ -64207,25 +64196,25 @@
         <v>9</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>194</v>
+        <v>170</v>
       </c>
       <c r="E15" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="F15">
         <v>13</v>
       </c>
       <c r="G15">
-        <f t="shared" si="2"/>
-        <v>0.20512820512820512</v>
+        <f>E15/$E$3</f>
+        <v>0.23076923076923078</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
-        <v>0.90308998699194354</v>
+        <f>LOG10(E15)</f>
+        <v>0.95424250943932487</v>
       </c>
       <c r="I15">
-        <f t="shared" si="1"/>
-        <v>0.56760107855061015</v>
+        <f>H15/$H$3</f>
+        <v>0.59975094991440026</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
@@ -64236,7 +64225,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>76</v>
+        <v>194</v>
       </c>
       <c r="E16" s="8">
         <v>8</v>
@@ -64245,15 +64234,15 @@
         <v>14</v>
       </c>
       <c r="G16">
-        <f t="shared" si="2"/>
+        <f>E16/$E$3</f>
         <v>0.20512820512820512</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f>LOG10(E16)</f>
         <v>0.90308998699194354</v>
       </c>
       <c r="I16">
-        <f t="shared" si="1"/>
+        <f>H16/$H$3</f>
         <v>0.56760107855061015</v>
       </c>
     </row>
@@ -64265,25 +64254,25 @@
         <v>4</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="E17" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F17">
         <v>15</v>
       </c>
       <c r="G17">
-        <f t="shared" si="2"/>
-        <v>0.17948717948717949</v>
+        <f>E17/$E$3</f>
+        <v>0.20512820512820512</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
-        <v>0.84509804001425681</v>
+        <f>LOG10(E17)</f>
+        <v>0.90308998699194354</v>
       </c>
       <c r="I17">
-        <f t="shared" si="1"/>
-        <v>0.53115256054475335</v>
+        <f>H17/$H$3</f>
+        <v>0.56760107855061015</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -64303,15 +64292,15 @@
         <v>16</v>
       </c>
       <c r="G18">
-        <f t="shared" si="2"/>
+        <f>E18/$E$3</f>
         <v>0.17948717948717949</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f>LOG10(E18)</f>
         <v>0.84509804001425681</v>
       </c>
       <c r="I18">
-        <f t="shared" si="1"/>
+        <f>H18/$H$3</f>
         <v>0.53115256054475335</v>
       </c>
     </row>
@@ -64332,15 +64321,15 @@
         <v>17</v>
       </c>
       <c r="G19">
-        <f t="shared" si="2"/>
+        <f>E19/$E$3</f>
         <v>0.17948717948717949</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f>LOG10(E19)</f>
         <v>0.84509804001425681</v>
       </c>
       <c r="I19">
-        <f t="shared" si="1"/>
+        <f>H19/$H$3</f>
         <v>0.53115256054475335</v>
       </c>
     </row>
@@ -64361,15 +64350,15 @@
         <v>18</v>
       </c>
       <c r="G20">
-        <f t="shared" si="2"/>
+        <f>E20/$E$3</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f>LOG10(E20)</f>
         <v>0.77815125038364363</v>
       </c>
       <c r="I20">
-        <f t="shared" si="1"/>
+        <f>H20/$H$3</f>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64390,15 +64379,15 @@
         <v>19</v>
       </c>
       <c r="G21">
-        <f t="shared" si="2"/>
+        <f>E21/$E$3</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f>LOG10(E21)</f>
         <v>0.77815125038364363</v>
       </c>
       <c r="I21">
-        <f t="shared" si="1"/>
+        <f>H21/$H$3</f>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64419,15 +64408,15 @@
         <v>20</v>
       </c>
       <c r="G22">
-        <f t="shared" si="2"/>
+        <f>E22/$E$3</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f>LOG10(E22)</f>
         <v>0.77815125038364363</v>
       </c>
       <c r="I22">
-        <f t="shared" si="1"/>
+        <f>H22/$H$3</f>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64448,15 +64437,15 @@
         <v>21</v>
       </c>
       <c r="G23">
-        <f t="shared" si="2"/>
+        <f>E23/$E$3</f>
         <v>0.15384615384615385</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f>LOG10(E23)</f>
         <v>0.77815125038364363</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f>H23/$H$3</f>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64477,15 +64466,15 @@
         <v>22</v>
       </c>
       <c r="G24">
-        <f t="shared" si="2"/>
+        <f>E24/$E$3</f>
         <v>0.12820512820512819</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f>LOG10(E24)</f>
         <v>0.69897000433601886</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f>H24/$H$3</f>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64506,15 +64495,15 @@
         <v>23</v>
       </c>
       <c r="G25">
-        <f t="shared" si="2"/>
+        <f>E25/$E$3</f>
         <v>0.12820512820512819</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
+        <f>LOG10(E25)</f>
         <v>0.69897000433601886</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f>H25/$H$3</f>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64526,7 +64515,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>256</v>
+        <v>177</v>
       </c>
       <c r="E26" s="8">
         <v>5</v>
@@ -64535,15 +64524,15 @@
         <v>24</v>
       </c>
       <c r="G26">
-        <f t="shared" si="2"/>
+        <f>E26/$E$3</f>
         <v>0.12820512820512819</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f>LOG10(E26)</f>
         <v>0.69897000433601886</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f>H26/$H$3</f>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64555,25 +64544,25 @@
         <v>4</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>177</v>
+        <v>91</v>
       </c>
       <c r="E27" s="8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F27">
         <v>25</v>
       </c>
       <c r="G27">
-        <f t="shared" si="2"/>
-        <v>0.12820512820512819</v>
+        <f>E27/$E$3</f>
+        <v>0.10256410256410256</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
-        <v>0.69897000433601886</v>
+        <f>LOG10(E27)</f>
+        <v>0.6020599913279624</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
-        <v>0.43930963032501014</v>
+        <f>H27/$H$3</f>
+        <v>0.37840071903374012</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -64584,7 +64573,7 @@
         <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>91</v>
+        <v>137</v>
       </c>
       <c r="E28" s="8">
         <v>4</v>
@@ -64593,15 +64582,15 @@
         <v>26</v>
       </c>
       <c r="G28">
-        <f t="shared" si="2"/>
+        <f>E28/$E$3</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f>LOG10(E28)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
+        <f>H28/$H$3</f>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64613,7 +64602,7 @@
         <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="E29" s="8">
         <v>4</v>
@@ -64622,15 +64611,15 @@
         <v>27</v>
       </c>
       <c r="G29">
-        <f t="shared" si="2"/>
+        <f>E29/$E$3</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="H29">
-        <f t="shared" si="0"/>
+        <f>LOG10(E29)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
+        <f>H29/$H$3</f>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64642,7 +64631,7 @@
         <v>4</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>160</v>
+        <v>168</v>
       </c>
       <c r="E30" s="8">
         <v>4</v>
@@ -64651,15 +64640,15 @@
         <v>28</v>
       </c>
       <c r="G30">
-        <f t="shared" si="2"/>
+        <f>E30/$E$3</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="H30">
-        <f t="shared" si="0"/>
+        <f>LOG10(E30)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f>H30/$H$3</f>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64671,7 +64660,7 @@
         <v>2</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>168</v>
+        <v>260</v>
       </c>
       <c r="E31" s="8">
         <v>4</v>
@@ -64680,15 +64669,15 @@
         <v>29</v>
       </c>
       <c r="G31">
-        <f t="shared" si="2"/>
+        <f>E31/$E$3</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="H31">
-        <f t="shared" si="0"/>
+        <f>LOG10(E31)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f>H31/$H$3</f>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64700,7 +64689,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>260</v>
+        <v>151</v>
       </c>
       <c r="E32" s="8">
         <v>4</v>
@@ -64709,19 +64698,19 @@
         <v>30</v>
       </c>
       <c r="G32">
-        <f t="shared" si="2"/>
+        <f>E32/$E$3</f>
         <v>0.10256410256410256</v>
       </c>
       <c r="H32">
-        <f t="shared" si="0"/>
+        <f>LOG10(E32)</f>
         <v>0.6020599913279624</v>
       </c>
       <c r="I32">
-        <f t="shared" si="1"/>
+        <f>H32/$H$3</f>
         <v>0.37840071903374012</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>244</v>
       </c>
@@ -64729,28 +64718,28 @@
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="E33" s="8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F33">
         <v>31</v>
       </c>
       <c r="G33">
-        <f t="shared" si="2"/>
-        <v>0.10256410256410256</v>
+        <f>E33/$E$3</f>
+        <v>7.6923076923076927E-2</v>
       </c>
       <c r="H33">
-        <f t="shared" si="0"/>
-        <v>0.6020599913279624</v>
+        <f>LOG10(E33)</f>
+        <v>0.47712125471966244</v>
       </c>
       <c r="I33">
-        <f t="shared" si="1"/>
-        <v>0.37840071903374012</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H33/$H$3</f>
+        <v>0.29987547495720013</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>714</v>
       </c>
@@ -64758,7 +64747,7 @@
         <v>38</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="E34" s="8">
         <v>3</v>
@@ -64767,19 +64756,19 @@
         <v>32</v>
       </c>
       <c r="G34">
-        <f t="shared" si="2"/>
+        <f>E34/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H34">
-        <f t="shared" si="0"/>
+        <f>LOG10(E34)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I34">
-        <f t="shared" si="1"/>
+        <f>H34/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -64787,7 +64776,7 @@
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>147</v>
+        <v>33</v>
       </c>
       <c r="E35" s="8">
         <v>3</v>
@@ -64796,19 +64785,19 @@
         <v>33</v>
       </c>
       <c r="G35">
-        <f t="shared" si="2"/>
+        <f>E35/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H35">
-        <f t="shared" si="0"/>
+        <f>LOG10(E35)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I35">
-        <f t="shared" si="1"/>
+        <f>H35/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>164</v>
       </c>
@@ -64816,7 +64805,7 @@
         <v>7</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>33</v>
+        <v>244</v>
       </c>
       <c r="E36" s="8">
         <v>3</v>
@@ -64825,19 +64814,22 @@
         <v>34</v>
       </c>
       <c r="G36">
-        <f t="shared" si="2"/>
+        <f>E36/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H36">
-        <f t="shared" si="0"/>
+        <f>LOG10(E36)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I36">
-        <f t="shared" si="1"/>
+        <f>H36/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M36" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>81</v>
       </c>
@@ -64845,7 +64837,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>244</v>
+        <v>191</v>
       </c>
       <c r="E37" s="8">
         <v>3</v>
@@ -64854,19 +64846,22 @@
         <v>35</v>
       </c>
       <c r="G37">
-        <f t="shared" si="2"/>
+        <f>E37/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H37">
-        <f t="shared" si="0"/>
+        <f>LOG10(E37)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I37">
-        <f t="shared" si="1"/>
+        <f>H37/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M37" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>191</v>
       </c>
@@ -64874,7 +64869,7 @@
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>191</v>
+        <v>141</v>
       </c>
       <c r="E38" s="8">
         <v>3</v>
@@ -64883,19 +64878,22 @@
         <v>36</v>
       </c>
       <c r="G38">
-        <f t="shared" si="2"/>
+        <f>E38/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H38">
-        <f t="shared" si="0"/>
+        <f>LOG10(E38)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I38">
-        <f t="shared" si="1"/>
+        <f>H38/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="M38" t="s">
+        <v>802</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -64903,7 +64901,7 @@
         <v>1</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>141</v>
+        <v>174</v>
       </c>
       <c r="E39" s="8">
         <v>3</v>
@@ -64912,19 +64910,19 @@
         <v>37</v>
       </c>
       <c r="G39">
-        <f t="shared" si="2"/>
+        <f>E39/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H39">
-        <f t="shared" si="0"/>
+        <f>LOG10(E39)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I39">
-        <f t="shared" si="1"/>
+        <f>H39/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>222</v>
       </c>
@@ -64932,7 +64930,7 @@
         <v>10</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>174</v>
+        <v>103</v>
       </c>
       <c r="E40" s="8">
         <v>3</v>
@@ -64941,19 +64939,19 @@
         <v>38</v>
       </c>
       <c r="G40">
-        <f t="shared" si="2"/>
+        <f>E40/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H40">
-        <f t="shared" si="0"/>
+        <f>LOG10(E40)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I40">
-        <f t="shared" si="1"/>
+        <f>H40/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>141</v>
       </c>
@@ -64961,28 +64959,28 @@
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E41" s="8">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F41">
         <v>39</v>
       </c>
       <c r="G41">
-        <f t="shared" si="2"/>
-        <v>7.6923076923076927E-2</v>
+        <f>E41/$E$3</f>
+        <v>5.128205128205128E-2</v>
       </c>
       <c r="H41">
-        <f t="shared" si="0"/>
-        <v>0.47712125471966244</v>
+        <f>LOG10(E41)</f>
+        <v>0.3010299956639812</v>
       </c>
       <c r="I41">
-        <f t="shared" si="1"/>
-        <v>0.29987547495720013</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+        <f>H41/$H$3</f>
+        <v>0.18920035951687006</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>784</v>
       </c>
@@ -64990,7 +64988,7 @@
         <v>2</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="E42" s="8">
         <v>2</v>
@@ -64999,19 +64997,19 @@
         <v>40</v>
       </c>
       <c r="G42">
-        <f t="shared" si="2"/>
+        <f>E42/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H42">
-        <f t="shared" si="0"/>
+        <f>LOG10(E42)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I42">
-        <f t="shared" si="1"/>
+        <f>H42/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>84</v>
       </c>
@@ -65019,7 +65017,7 @@
         <v>6</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>98</v>
+        <v>121</v>
       </c>
       <c r="E43" s="8">
         <v>2</v>
@@ -65028,19 +65026,19 @@
         <v>41</v>
       </c>
       <c r="G43">
-        <f t="shared" si="2"/>
+        <f>E43/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H43">
-        <f t="shared" si="0"/>
+        <f>LOG10(E43)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I43">
-        <f t="shared" si="1"/>
+        <f>H43/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>260</v>
       </c>
@@ -65048,7 +65046,7 @@
         <v>4</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>121</v>
+        <v>53</v>
       </c>
       <c r="E44" s="8">
         <v>2</v>
@@ -65057,19 +65055,19 @@
         <v>42</v>
       </c>
       <c r="G44">
-        <f t="shared" si="2"/>
+        <f>E44/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H44">
-        <f t="shared" si="0"/>
+        <f>LOG10(E44)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I44">
-        <f t="shared" si="1"/>
+        <f>H44/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>256</v>
       </c>
@@ -65077,7 +65075,7 @@
         <v>5</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>53</v>
+        <v>100</v>
       </c>
       <c r="E45" s="8">
         <v>2</v>
@@ -65086,19 +65084,19 @@
         <v>43</v>
       </c>
       <c r="G45">
-        <f t="shared" si="2"/>
+        <f>E45/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H45">
-        <f t="shared" si="0"/>
+        <f>LOG10(E45)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I45">
-        <f t="shared" si="1"/>
+        <f>H45/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>170</v>
       </c>
@@ -65106,7 +65104,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>100</v>
+        <v>45</v>
       </c>
       <c r="E46" s="8">
         <v>2</v>
@@ -65115,19 +65113,19 @@
         <v>44</v>
       </c>
       <c r="G46">
-        <f t="shared" si="2"/>
+        <f>E46/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H46">
-        <f t="shared" si="0"/>
+        <f>LOG10(E46)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I46">
-        <f t="shared" si="1"/>
+        <f>H46/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>174</v>
       </c>
@@ -65135,7 +65133,7 @@
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>45</v>
+        <v>784</v>
       </c>
       <c r="E47" s="8">
         <v>2</v>
@@ -65144,19 +65142,19 @@
         <v>45</v>
       </c>
       <c r="G47">
-        <f t="shared" si="2"/>
+        <f>E47/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H47">
-        <f t="shared" si="0"/>
+        <f>LOG10(E47)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I47">
-        <f t="shared" si="1"/>
+        <f>H47/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>110</v>
       </c>
@@ -65164,7 +65162,7 @@
         <v>17</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>784</v>
+        <v>265</v>
       </c>
       <c r="E48" s="8">
         <v>2</v>
@@ -65173,15 +65171,15 @@
         <v>46</v>
       </c>
       <c r="G48">
-        <f t="shared" si="2"/>
+        <f>E48/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H48">
-        <f t="shared" si="0"/>
+        <f>LOG10(E48)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I48">
-        <f t="shared" si="1"/>
+        <f>H48/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65193,7 +65191,7 @@
         <v>4</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="E49" s="8">
         <v>2</v>
@@ -65202,15 +65200,15 @@
         <v>47</v>
       </c>
       <c r="G49">
-        <f t="shared" si="2"/>
+        <f>E49/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H49">
-        <f t="shared" si="0"/>
+        <f>LOG10(E49)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I49">
-        <f t="shared" si="1"/>
+        <f>H49/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65222,7 +65220,7 @@
         <v>7</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>269</v>
+        <v>189</v>
       </c>
       <c r="E50" s="8">
         <v>2</v>
@@ -65231,15 +65229,15 @@
         <v>48</v>
       </c>
       <c r="G50">
-        <f t="shared" si="2"/>
+        <f>E50/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H50">
-        <f t="shared" si="0"/>
+        <f>LOG10(E50)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I50">
-        <f t="shared" si="1"/>
+        <f>H50/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65251,7 +65249,7 @@
         <v>6</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>189</v>
+        <v>57</v>
       </c>
       <c r="E51" s="8">
         <v>2</v>
@@ -65260,15 +65258,15 @@
         <v>49</v>
       </c>
       <c r="G51">
-        <f t="shared" si="2"/>
+        <f>E51/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H51">
-        <f t="shared" si="0"/>
+        <f>LOG10(E51)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I51">
-        <f t="shared" si="1"/>
+        <f>H51/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65280,7 +65278,7 @@
         <v>7</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>57</v>
+        <v>156</v>
       </c>
       <c r="E52" s="8">
         <v>2</v>
@@ -65289,15 +65287,15 @@
         <v>50</v>
       </c>
       <c r="G52">
-        <f t="shared" si="2"/>
+        <f>E52/$E$3</f>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H52">
-        <f t="shared" si="0"/>
+        <f>LOG10(E52)</f>
         <v>0.3010299956639812</v>
       </c>
       <c r="I52">
-        <f t="shared" si="1"/>
+        <f>H52/$H$3</f>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65309,25 +65307,25 @@
         <v>8</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>156</v>
+        <v>208</v>
       </c>
       <c r="E53" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F53">
         <v>51</v>
       </c>
       <c r="G53">
-        <f t="shared" si="2"/>
-        <v>5.128205128205128E-2</v>
+        <f>E53/$E$3</f>
+        <v>2.564102564102564E-2</v>
       </c>
       <c r="H53">
-        <f t="shared" si="0"/>
-        <v>0.3010299956639812</v>
+        <f>LOG10(E53)</f>
+        <v>0</v>
       </c>
       <c r="I53">
-        <f t="shared" si="1"/>
-        <v>0.18920035951687006</v>
+        <f>H53/$H$3</f>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
@@ -65338,7 +65336,7 @@
         <v>2</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>208</v>
+        <v>272</v>
       </c>
       <c r="E54" s="8">
         <v>1</v>
@@ -65347,15 +65345,15 @@
         <v>52</v>
       </c>
       <c r="G54">
-        <f t="shared" si="2"/>
+        <f>E54/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H54">
-        <f t="shared" si="0"/>
+        <f>LOG10(E54)</f>
         <v>0</v>
       </c>
       <c r="I54">
-        <f t="shared" si="1"/>
+        <f>H54/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65367,7 +65365,7 @@
         <v>2</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>272</v>
+        <v>107</v>
       </c>
       <c r="E55" s="8">
         <v>1</v>
@@ -65376,15 +65374,15 @@
         <v>53</v>
       </c>
       <c r="G55">
-        <f t="shared" si="2"/>
+        <f>E55/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H55">
-        <f t="shared" si="0"/>
+        <f>LOG10(E55)</f>
         <v>0</v>
       </c>
       <c r="I55">
-        <f t="shared" si="1"/>
+        <f>H55/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65396,7 +65394,7 @@
         <v>8</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>107</v>
+        <v>252</v>
       </c>
       <c r="E56" s="8">
         <v>1</v>
@@ -65405,15 +65403,15 @@
         <v>54</v>
       </c>
       <c r="G56">
-        <f t="shared" si="2"/>
+        <f>E56/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H56">
-        <f t="shared" si="0"/>
+        <f>LOG10(E56)</f>
         <v>0</v>
       </c>
       <c r="I56">
-        <f t="shared" si="1"/>
+        <f>H56/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65425,7 +65423,7 @@
         <v>5</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>241</v>
+        <v>117</v>
       </c>
       <c r="E57" s="8">
         <v>1</v>
@@ -65434,15 +65432,15 @@
         <v>55</v>
       </c>
       <c r="G57">
-        <f t="shared" si="2"/>
+        <f>E57/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H57">
-        <f t="shared" si="0"/>
+        <f>LOG10(E57)</f>
         <v>0</v>
       </c>
       <c r="I57">
-        <f t="shared" si="1"/>
+        <f>H57/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65454,7 +65452,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>213</v>
+        <v>81</v>
       </c>
       <c r="E58" s="8">
         <v>1</v>
@@ -65463,15 +65461,15 @@
         <v>56</v>
       </c>
       <c r="G58">
-        <f t="shared" si="2"/>
+        <f>E58/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H58">
-        <f t="shared" si="0"/>
+        <f>LOG10(E58)</f>
         <v>0</v>
       </c>
       <c r="I58">
-        <f t="shared" si="1"/>
+        <f>H58/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65483,7 +65481,7 @@
         <v>2</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>252</v>
+        <v>39</v>
       </c>
       <c r="E59" s="8">
         <v>1</v>
@@ -65492,15 +65490,15 @@
         <v>57</v>
       </c>
       <c r="G59">
-        <f t="shared" si="2"/>
+        <f>E59/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H59">
-        <f t="shared" si="0"/>
+        <f>LOG10(E59)</f>
         <v>0</v>
       </c>
       <c r="I59">
-        <f t="shared" si="1"/>
+        <f>H59/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65512,7 +65510,7 @@
         <v>2</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="E60" s="8">
         <v>1</v>
@@ -65521,15 +65519,15 @@
         <v>58</v>
       </c>
       <c r="G60">
-        <f t="shared" si="2"/>
+        <f>E60/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H60">
-        <f t="shared" si="0"/>
+        <f>LOG10(E60)</f>
         <v>0</v>
       </c>
       <c r="I60">
-        <f t="shared" si="1"/>
+        <f>H60/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65541,7 +65539,7 @@
         <v>2</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="E61" s="8">
         <v>1</v>
@@ -65550,15 +65548,15 @@
         <v>59</v>
       </c>
       <c r="G61">
-        <f t="shared" si="2"/>
+        <f>E61/$E$3</f>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H61">
-        <f t="shared" si="0"/>
+        <f>LOG10(E61)</f>
         <v>0</v>
       </c>
       <c r="I61">
-        <f t="shared" si="1"/>
+        <f>H61/$H$3</f>
         <v>0</v>
       </c>
     </row>
@@ -65569,27 +65567,6 @@
       <c r="B62" s="8">
         <v>1</v>
       </c>
-      <c r="D62" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E62" s="8">
-        <v>1</v>
-      </c>
-      <c r="F62">
-        <v>60</v>
-      </c>
-      <c r="G62">
-        <f t="shared" si="2"/>
-        <v>2.564102564102564E-2</v>
-      </c>
-      <c r="H62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I62">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
@@ -65598,27 +65575,6 @@
       <c r="B63" s="8">
         <v>1</v>
       </c>
-      <c r="D63" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="E63" s="8">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>61</v>
-      </c>
-      <c r="G63">
-        <f t="shared" si="2"/>
-        <v>2.564102564102564E-2</v>
-      </c>
-      <c r="H63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I63">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
@@ -65627,27 +65583,6 @@
       <c r="B64" s="8">
         <v>20</v>
       </c>
-      <c r="D64" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E64" s="8">
-        <v>1</v>
-      </c>
-      <c r="F64">
-        <v>62</v>
-      </c>
-      <c r="G64">
-        <f t="shared" si="2"/>
-        <v>2.564102564102564E-2</v>
-      </c>
-      <c r="H64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I64">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
@@ -65666,8 +65601,9 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:F64">
-    <sortCondition descending="1" ref="E3"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:I61">
+    <sortCondition descending="1" ref="E3:E61"/>
+    <sortCondition ref="D3:D61"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
updat N. validoi subadult
</commit_message>
<xml_diff>
--- a/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
+++ b/data/raw/GranCanaria_ES_TOTAL_v1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WARD\OneDrive - UGent\School\1ste master\sem_2\Project\landsnails-occurrences\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1490" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{86923AF8-88F6-481E-9EF6-2FB48909B3A5}"/>
+  <xr:revisionPtr revIDLastSave="1498" documentId="11_F25DC773A252ABDACC10485D49DE6EB05ADE58E7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C08966BE-2449-484C-A171-A36300E172AB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,16 @@
     <sheet name="spec per gen" sheetId="11" r:id="rId5"/>
     <sheet name="taxa_abundance" sheetId="13" r:id="rId6"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId7"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">genus!$D$2:$E$28</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AG$390</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId8"/>
-    <pivotCache cacheId="1" r:id="rId9"/>
-    <pivotCache cacheId="2" r:id="rId10"/>
-    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId10"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -51,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8673" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8676" uniqueCount="804">
   <si>
     <t>orderNumber</t>
   </si>
@@ -2460,6 +2457,9 @@
   </si>
   <si>
     <t>Hemicycla psathyra cf. temperata samen met Hemicycla psathyra temperata</t>
+  </si>
+  <si>
+    <t>subadult</t>
   </si>
 </sst>
 </file>
@@ -3382,7 +3382,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{25B91953-E372-43CC-AB90-FC353682EE4E}" type="CELLRANGE">
+                    <a:fld id="{F4AF2FD3-BE36-41F2-9495-69133F092083}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3416,7 +3416,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E41F9129-A823-4AE6-9228-BC780F67B094}" type="CELLRANGE">
+                    <a:fld id="{50A041CC-D57A-4B3C-89BE-B2E914886BD0}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3450,7 +3450,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C0A8722F-610C-4285-92E9-F56F498F06FB}" type="CELLRANGE">
+                    <a:fld id="{8B48BA8D-EBE2-49E7-881C-4CFDAA4BAC09}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3484,7 +3484,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CC4876FC-ABCB-4B0E-B7BF-4A8460DBDF12}" type="CELLRANGE">
+                    <a:fld id="{05F3F967-2C42-4766-B621-0AEF498CF149}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3518,7 +3518,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{71F3D7F4-68C5-48BE-95B2-7301A392C45A}" type="CELLRANGE">
+                    <a:fld id="{E4BB4228-86EF-4BE3-8CB1-946611B79236}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3552,7 +3552,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{340B1BD6-B59E-4026-AE1F-FA47AEDADB2A}" type="CELLRANGE">
+                    <a:fld id="{25514F45-CA4A-42BD-A23E-12D0F894E643}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3586,7 +3586,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{94F21806-E123-4F29-AE87-205DAA8080BB}" type="CELLRANGE">
+                    <a:fld id="{5A3B9E06-CDC9-4950-A883-85DDC2FC22B3}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3620,7 +3620,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{AFA593F8-6B10-4C8F-A2D6-156DB5557C10}" type="CELLRANGE">
+                    <a:fld id="{2B61DAC0-83CD-43DD-AA75-1CC8EAD69C0D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3654,7 +3654,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{7014CC1B-8843-48FE-9EE9-BF399E85B890}" type="CELLRANGE">
+                    <a:fld id="{0C53EC9B-0F91-4083-BAF8-AFEFF90EFF64}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3688,7 +3688,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BFDCD56A-F8C2-4F28-8D45-54E492046558}" type="CELLRANGE">
+                    <a:fld id="{AFEB7603-9F66-4686-9AB5-89C81C3F5BF1}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3722,7 +3722,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{DDA29EE2-6602-4008-99C8-82020063E827}" type="CELLRANGE">
+                    <a:fld id="{A99C7C28-8D19-43D8-A5BD-884537F0366B}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3756,7 +3756,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{0812A2CE-20D4-435F-A02B-BF6C0CCD6A33}" type="CELLRANGE">
+                    <a:fld id="{FD00ACCB-654E-4BE6-8E32-97DA5B9DF2E2}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3790,7 +3790,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{CB234CE2-9783-4970-A6C5-D467FBF21B94}" type="CELLRANGE">
+                    <a:fld id="{2041B65D-1BDD-4D38-8115-E3A96F83B812}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3824,7 +3824,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C4F4F44B-FD03-4172-8A83-8F62B39ED0A3}" type="CELLRANGE">
+                    <a:fld id="{B4834152-585D-483C-80C6-3F0BE281E3FC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3858,7 +3858,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{4A56BC14-A834-40F4-9345-4645D8A87CD6}" type="CELLRANGE">
+                    <a:fld id="{F2139E63-AFDE-4984-AA62-B170CC964FDC}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3892,7 +3892,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A0E2E6C5-11CB-41FC-8B6D-BCBA91B875FB}" type="CELLRANGE">
+                    <a:fld id="{53A11B47-3DC5-4C7A-924A-3BBC3FE06155}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3926,7 +3926,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{B1D9611D-8318-40D6-A8BD-343F584A0DF7}" type="CELLRANGE">
+                    <a:fld id="{A2A7F9D1-C82B-425E-8118-4125436428C5}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3960,7 +3960,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9C3F4A9B-56E4-4066-B15D-F2B829EE7E11}" type="CELLRANGE">
+                    <a:fld id="{CE330D85-3D56-47F8-AD56-8A532AE19A05}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3994,7 +3994,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{5BA7F935-40E1-4837-9467-66FF352EBC5D}" type="CELLRANGE">
+                    <a:fld id="{917B4C06-9ABC-447B-BD1D-F9D068066818}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4028,7 +4028,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{A7C4C672-2C5F-4546-A98D-A77F6BD9F09F}" type="CELLRANGE">
+                    <a:fld id="{6BE9863B-0287-4DEA-AC87-315B70EE9A6D}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4062,7 +4062,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{837DBB51-7AC6-44CF-B520-7D4E5F1B2D62}" type="CELLRANGE">
+                    <a:fld id="{4438D1C6-87D6-4DC8-84EF-5DBC3192B937}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4096,7 +4096,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{F460A83D-1D79-44DA-8F78-20BDF3A7BB86}" type="CELLRANGE">
+                    <a:fld id="{D4409010-BD88-468C-B909-EDD2B07DBB4E}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4130,7 +4130,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{30A842FD-8A4C-4DAD-82A1-F319501F70BD}" type="CELLRANGE">
+                    <a:fld id="{79B5C9CD-8E56-4388-A71F-AC7896033DB4}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4164,7 +4164,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{64D6E44F-6AA7-460B-A00F-A0767A8819E7}" type="CELLRANGE">
+                    <a:fld id="{0BCBD8DA-0FCD-4831-9117-A6F650AF3363}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4198,7 +4198,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{9894C4A2-9D04-4667-BB6F-8468DCCDD13D}" type="CELLRANGE">
+                    <a:fld id="{FD4C78D0-C4E5-4211-A537-F68A79E6E501}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4232,7 +4232,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C18E3EF6-3B35-4D71-A2AC-CDC491D0AAC3}" type="CELLRANGE">
+                    <a:fld id="{7EFF41CF-BC13-437B-800F-98A80674B169}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -4266,7 +4266,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{686F1EF0-DB0D-43A0-9C42-E4180A2675E7}" type="CELLRANGE">
+                    <a:fld id="{EB5A57ED-4876-4767-B33E-F26C19792B95}" type="CELLRANGE">
                       <a:rPr lang="en-GB"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -8930,19 +8930,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet7"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="WARD" refreshedDate="43891.590313078705" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="390" xr:uid="{869674DF-0315-4FAD-B166-8FA90FD916D1}">
   <cacheSource type="worksheet">
@@ -26477,8 +26464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG390"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A355" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AE382" sqref="AE382"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -57009,7 +56996,7 @@
         <v>688</v>
       </c>
       <c r="M351" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="N351" s="1">
         <v>4</v>
@@ -57061,6 +57048,9 @@
       </c>
       <c r="AD351" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="AE351" s="1" t="s">
+        <v>803</v>
       </c>
       <c r="AF351" s="1" t="s">
         <v>706</v>
@@ -58287,7 +58277,7 @@
         <v>688</v>
       </c>
       <c r="M365" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="N365" s="1">
         <v>2</v>
@@ -58339,6 +58329,9 @@
       </c>
       <c r="AD365" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="AE365" s="1" t="s">
+        <v>803</v>
       </c>
       <c r="AF365" s="1" t="s">
         <v>706</v>
@@ -59773,7 +59766,7 @@
         <v>688</v>
       </c>
       <c r="M382" s="1" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="N382" s="1">
         <v>1</v>
@@ -59825,6 +59818,9 @@
       </c>
       <c r="AD382" s="1" t="s">
         <v>29</v>
+      </c>
+      <c r="AE382" s="1" t="s">
+        <v>803</v>
       </c>
       <c r="AF382" s="1" t="s">
         <v>706</v>
@@ -63807,7 +63803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29377B9E-EE4F-45EE-ABD5-75334AF19FBC}">
   <dimension ref="A2:M66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+    <sheetView topLeftCell="D16" workbookViewId="0">
       <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
@@ -63857,15 +63853,15 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>E3/$E$3</f>
+        <f t="shared" ref="G3:G34" si="0">E3/$E$3</f>
         <v>1</v>
       </c>
       <c r="H3">
-        <f>LOG10(E3)</f>
+        <f t="shared" ref="H3:H34" si="1">LOG10(E3)</f>
         <v>1.5910646070264991</v>
       </c>
       <c r="I3">
-        <f>H3/$H$3</f>
+        <f t="shared" ref="I3:I34" si="2">H3/$H$3</f>
         <v>1</v>
       </c>
     </row>
@@ -63886,15 +63882,15 @@
         <v>2</v>
       </c>
       <c r="G4">
-        <f>E4/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.97435897435897434</v>
       </c>
       <c r="H4">
-        <f>LOG10(E4)</f>
+        <f t="shared" si="1"/>
         <v>1.5797835966168101</v>
       </c>
       <c r="I4">
-        <f>H4/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.99290977226200028</v>
       </c>
     </row>
@@ -63915,15 +63911,15 @@
         <v>3</v>
       </c>
       <c r="G5">
-        <f>E5/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.76923076923076927</v>
       </c>
       <c r="H5">
-        <f>LOG10(E5)</f>
+        <f t="shared" si="1"/>
         <v>1.4771212547196624</v>
       </c>
       <c r="I5">
-        <f>H5/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.92838546479908024</v>
       </c>
     </row>
@@ -63944,15 +63940,15 @@
         <v>4</v>
       </c>
       <c r="G6">
-        <f>E6/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.53846153846153844</v>
       </c>
       <c r="H6">
-        <f>LOG10(E6)</f>
+        <f t="shared" si="1"/>
         <v>1.3222192947339193</v>
       </c>
       <c r="I6">
-        <f>H6/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.83102803550195359</v>
       </c>
     </row>
@@ -63973,15 +63969,15 @@
         <v>5</v>
       </c>
       <c r="G7">
-        <f>E7/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.51282051282051277</v>
       </c>
       <c r="H7">
-        <f>LOG10(E7)</f>
+        <f t="shared" si="1"/>
         <v>1.3010299956639813</v>
       </c>
       <c r="I7">
-        <f>H7/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.8177103493587502</v>
       </c>
     </row>
@@ -64002,15 +63998,15 @@
         <v>6</v>
       </c>
       <c r="G8">
-        <f>E8/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.4358974358974359</v>
       </c>
       <c r="H8">
-        <f>LOG10(E8)</f>
+        <f t="shared" si="1"/>
         <v>1.2304489213782739</v>
       </c>
       <c r="I8">
-        <f>H8/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.77334943907641129</v>
       </c>
     </row>
@@ -64031,15 +64027,15 @@
         <v>7</v>
       </c>
       <c r="G9">
-        <f>E9/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.35897435897435898</v>
       </c>
       <c r="H9">
-        <f>LOG10(E9)</f>
+        <f t="shared" si="1"/>
         <v>1.146128035678238</v>
       </c>
       <c r="I9">
-        <f>H9/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.72035292006162344</v>
       </c>
     </row>
@@ -64060,15 +64056,15 @@
         <v>8</v>
       </c>
       <c r="G10">
-        <f>E10/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.30769230769230771</v>
       </c>
       <c r="H10">
-        <f>LOG10(E10)</f>
+        <f t="shared" si="1"/>
         <v>1.0791812460476249</v>
       </c>
       <c r="I10">
-        <f>H10/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.6782761939909403</v>
       </c>
     </row>
@@ -64089,15 +64085,15 @@
         <v>9</v>
       </c>
       <c r="G11">
-        <f>E11/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.25641025641025639</v>
       </c>
       <c r="H11">
-        <f>LOG10(E11)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I11">
-        <f>H11/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.62850998984188011</v>
       </c>
     </row>
@@ -64118,15 +64114,15 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <f>E12/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.25641025641025639</v>
       </c>
       <c r="H12">
-        <f>LOG10(E12)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="I12">
-        <f>H12/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.62850998984188011</v>
       </c>
     </row>
@@ -64147,15 +64143,15 @@
         <v>11</v>
       </c>
       <c r="G13">
-        <f>E13/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="H13">
-        <f>LOG10(E13)</f>
+        <f t="shared" si="1"/>
         <v>0.95424250943932487</v>
       </c>
       <c r="I13">
-        <f>H13/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.59975094991440026</v>
       </c>
     </row>
@@ -64176,15 +64172,15 @@
         <v>12</v>
       </c>
       <c r="G14">
-        <f>E14/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="H14">
-        <f>LOG10(E14)</f>
+        <f t="shared" si="1"/>
         <v>0.95424250943932487</v>
       </c>
       <c r="I14">
-        <f>H14/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.59975094991440026</v>
       </c>
     </row>
@@ -64205,15 +64201,15 @@
         <v>13</v>
       </c>
       <c r="G15">
-        <f>E15/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.23076923076923078</v>
       </c>
       <c r="H15">
-        <f>LOG10(E15)</f>
+        <f t="shared" si="1"/>
         <v>0.95424250943932487</v>
       </c>
       <c r="I15">
-        <f>H15/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.59975094991440026</v>
       </c>
     </row>
@@ -64234,15 +64230,15 @@
         <v>14</v>
       </c>
       <c r="G16">
-        <f>E16/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.20512820512820512</v>
       </c>
       <c r="H16">
-        <f>LOG10(E16)</f>
+        <f t="shared" si="1"/>
         <v>0.90308998699194354</v>
       </c>
       <c r="I16">
-        <f>H16/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.56760107855061015</v>
       </c>
     </row>
@@ -64263,15 +64259,15 @@
         <v>15</v>
       </c>
       <c r="G17">
-        <f>E17/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.20512820512820512</v>
       </c>
       <c r="H17">
-        <f>LOG10(E17)</f>
+        <f t="shared" si="1"/>
         <v>0.90308998699194354</v>
       </c>
       <c r="I17">
-        <f>H17/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.56760107855061015</v>
       </c>
     </row>
@@ -64292,15 +64288,15 @@
         <v>16</v>
       </c>
       <c r="G18">
-        <f>E18/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.17948717948717949</v>
       </c>
       <c r="H18">
-        <f>LOG10(E18)</f>
+        <f t="shared" si="1"/>
         <v>0.84509804001425681</v>
       </c>
       <c r="I18">
-        <f>H18/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.53115256054475335</v>
       </c>
     </row>
@@ -64321,15 +64317,15 @@
         <v>17</v>
       </c>
       <c r="G19">
-        <f>E19/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.17948717948717949</v>
       </c>
       <c r="H19">
-        <f>LOG10(E19)</f>
+        <f t="shared" si="1"/>
         <v>0.84509804001425681</v>
       </c>
       <c r="I19">
-        <f>H19/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.53115256054475335</v>
       </c>
     </row>
@@ -64350,15 +64346,15 @@
         <v>18</v>
       </c>
       <c r="G20">
-        <f>E20/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="H20">
-        <f>LOG10(E20)</f>
+        <f t="shared" si="1"/>
         <v>0.77815125038364363</v>
       </c>
       <c r="I20">
-        <f>H20/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64379,15 +64375,15 @@
         <v>19</v>
       </c>
       <c r="G21">
-        <f>E21/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="H21">
-        <f>LOG10(E21)</f>
+        <f t="shared" si="1"/>
         <v>0.77815125038364363</v>
       </c>
       <c r="I21">
-        <f>H21/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64408,15 +64404,15 @@
         <v>20</v>
       </c>
       <c r="G22">
-        <f>E22/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="H22">
-        <f>LOG10(E22)</f>
+        <f t="shared" si="1"/>
         <v>0.77815125038364363</v>
       </c>
       <c r="I22">
-        <f>H22/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64437,15 +64433,15 @@
         <v>21</v>
       </c>
       <c r="G23">
-        <f>E23/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.15384615384615385</v>
       </c>
       <c r="H23">
-        <f>LOG10(E23)</f>
+        <f t="shared" si="1"/>
         <v>0.77815125038364363</v>
       </c>
       <c r="I23">
-        <f>H23/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.48907583447407021</v>
       </c>
     </row>
@@ -64466,15 +64462,15 @@
         <v>22</v>
       </c>
       <c r="G24">
-        <f>E24/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.12820512820512819</v>
       </c>
       <c r="H24">
-        <f>LOG10(E24)</f>
+        <f t="shared" si="1"/>
         <v>0.69897000433601886</v>
       </c>
       <c r="I24">
-        <f>H24/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64495,15 +64491,15 @@
         <v>23</v>
       </c>
       <c r="G25">
-        <f>E25/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.12820512820512819</v>
       </c>
       <c r="H25">
-        <f>LOG10(E25)</f>
+        <f t="shared" si="1"/>
         <v>0.69897000433601886</v>
       </c>
       <c r="I25">
-        <f>H25/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64524,15 +64520,15 @@
         <v>24</v>
       </c>
       <c r="G26">
-        <f>E26/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.12820512820512819</v>
       </c>
       <c r="H26">
-        <f>LOG10(E26)</f>
+        <f t="shared" si="1"/>
         <v>0.69897000433601886</v>
       </c>
       <c r="I26">
-        <f>H26/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.43930963032501014</v>
       </c>
     </row>
@@ -64553,15 +64549,15 @@
         <v>25</v>
       </c>
       <c r="G27">
-        <f>E27/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H27">
-        <f>LOG10(E27)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I27">
-        <f>H27/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64582,15 +64578,15 @@
         <v>26</v>
       </c>
       <c r="G28">
-        <f>E28/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H28">
-        <f>LOG10(E28)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I28">
-        <f>H28/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64611,15 +64607,15 @@
         <v>27</v>
       </c>
       <c r="G29">
-        <f>E29/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H29">
-        <f>LOG10(E29)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I29">
-        <f>H29/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64640,15 +64636,15 @@
         <v>28</v>
       </c>
       <c r="G30">
-        <f>E30/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H30">
-        <f>LOG10(E30)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I30">
-        <f>H30/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64669,15 +64665,15 @@
         <v>29</v>
       </c>
       <c r="G31">
-        <f>E31/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H31">
-        <f>LOG10(E31)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I31">
-        <f>H31/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64698,15 +64694,15 @@
         <v>30</v>
       </c>
       <c r="G32">
-        <f>E32/$E$3</f>
+        <f t="shared" si="0"/>
         <v>0.10256410256410256</v>
       </c>
       <c r="H32">
-        <f>LOG10(E32)</f>
+        <f t="shared" si="1"/>
         <v>0.6020599913279624</v>
       </c>
       <c r="I32">
-        <f>H32/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.37840071903374012</v>
       </c>
     </row>
@@ -64727,15 +64723,15 @@
         <v>31</v>
       </c>
       <c r="G33">
-        <f>E33/$E$3</f>
+        <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H33">
-        <f>LOG10(E33)</f>
+        <f t="shared" si="1"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I33">
-        <f>H33/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.29987547495720013</v>
       </c>
     </row>
@@ -64756,15 +64752,15 @@
         <v>32</v>
       </c>
       <c r="G34">
-        <f>E34/$E$3</f>
+        <f t="shared" si="0"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H34">
-        <f>LOG10(E34)</f>
+        <f t="shared" si="1"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I34">
-        <f>H34/$H$3</f>
+        <f t="shared" si="2"/>
         <v>0.29987547495720013</v>
       </c>
     </row>
@@ -64785,15 +64781,15 @@
         <v>33</v>
       </c>
       <c r="G35">
-        <f>E35/$E$3</f>
+        <f t="shared" ref="G35:G61" si="3">E35/$E$3</f>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H35">
-        <f>LOG10(E35)</f>
+        <f t="shared" ref="H35:H61" si="4">LOG10(E35)</f>
         <v>0.47712125471966244</v>
       </c>
       <c r="I35">
-        <f>H35/$H$3</f>
+        <f t="shared" ref="I35:I66" si="5">H35/$H$3</f>
         <v>0.29987547495720013</v>
       </c>
     </row>
@@ -64814,15 +64810,15 @@
         <v>34</v>
       </c>
       <c r="G36">
-        <f>E36/$E$3</f>
+        <f t="shared" si="3"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H36">
-        <f>LOG10(E36)</f>
+        <f t="shared" si="4"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I36">
-        <f>H36/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.29987547495720013</v>
       </c>
       <c r="M36" t="s">
@@ -64846,15 +64842,15 @@
         <v>35</v>
       </c>
       <c r="G37">
-        <f>E37/$E$3</f>
+        <f t="shared" si="3"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H37">
-        <f>LOG10(E37)</f>
+        <f t="shared" si="4"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I37">
-        <f>H37/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.29987547495720013</v>
       </c>
       <c r="M37" t="s">
@@ -64878,15 +64874,15 @@
         <v>36</v>
       </c>
       <c r="G38">
-        <f>E38/$E$3</f>
+        <f t="shared" si="3"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H38">
-        <f>LOG10(E38)</f>
+        <f t="shared" si="4"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I38">
-        <f>H38/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.29987547495720013</v>
       </c>
       <c r="M38" t="s">
@@ -64910,15 +64906,15 @@
         <v>37</v>
       </c>
       <c r="G39">
-        <f>E39/$E$3</f>
+        <f t="shared" si="3"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H39">
-        <f>LOG10(E39)</f>
+        <f t="shared" si="4"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I39">
-        <f>H39/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.29987547495720013</v>
       </c>
     </row>
@@ -64939,15 +64935,15 @@
         <v>38</v>
       </c>
       <c r="G40">
-        <f>E40/$E$3</f>
+        <f t="shared" si="3"/>
         <v>7.6923076923076927E-2</v>
       </c>
       <c r="H40">
-        <f>LOG10(E40)</f>
+        <f t="shared" si="4"/>
         <v>0.47712125471966244</v>
       </c>
       <c r="I40">
-        <f>H40/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.29987547495720013</v>
       </c>
     </row>
@@ -64968,15 +64964,15 @@
         <v>39</v>
       </c>
       <c r="G41">
-        <f>E41/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H41">
-        <f>LOG10(E41)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I41">
-        <f>H41/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -64997,15 +64993,15 @@
         <v>40</v>
       </c>
       <c r="G42">
-        <f>E42/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H42">
-        <f>LOG10(E42)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I42">
-        <f>H42/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65026,15 +65022,15 @@
         <v>41</v>
       </c>
       <c r="G43">
-        <f>E43/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H43">
-        <f>LOG10(E43)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I43">
-        <f>H43/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65055,15 +65051,15 @@
         <v>42</v>
       </c>
       <c r="G44">
-        <f>E44/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H44">
-        <f>LOG10(E44)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I44">
-        <f>H44/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65084,15 +65080,15 @@
         <v>43</v>
       </c>
       <c r="G45">
-        <f>E45/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H45">
-        <f>LOG10(E45)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I45">
-        <f>H45/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65113,15 +65109,15 @@
         <v>44</v>
       </c>
       <c r="G46">
-        <f>E46/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H46">
-        <f>LOG10(E46)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I46">
-        <f>H46/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65142,15 +65138,15 @@
         <v>45</v>
       </c>
       <c r="G47">
-        <f>E47/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H47">
-        <f>LOG10(E47)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I47">
-        <f>H47/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65171,15 +65167,15 @@
         <v>46</v>
       </c>
       <c r="G48">
-        <f>E48/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H48">
-        <f>LOG10(E48)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I48">
-        <f>H48/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65200,15 +65196,15 @@
         <v>47</v>
       </c>
       <c r="G49">
-        <f>E49/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H49">
-        <f>LOG10(E49)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I49">
-        <f>H49/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65229,15 +65225,15 @@
         <v>48</v>
       </c>
       <c r="G50">
-        <f>E50/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H50">
-        <f>LOG10(E50)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I50">
-        <f>H50/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65258,15 +65254,15 @@
         <v>49</v>
       </c>
       <c r="G51">
-        <f>E51/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H51">
-        <f>LOG10(E51)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I51">
-        <f>H51/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65287,15 +65283,15 @@
         <v>50</v>
       </c>
       <c r="G52">
-        <f>E52/$E$3</f>
+        <f t="shared" si="3"/>
         <v>5.128205128205128E-2</v>
       </c>
       <c r="H52">
-        <f>LOG10(E52)</f>
+        <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
       <c r="I52">
-        <f>H52/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0.18920035951687006</v>
       </c>
     </row>
@@ -65316,15 +65312,15 @@
         <v>51</v>
       </c>
       <c r="G53">
-        <f>E53/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H53">
-        <f>LOG10(E53)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I53">
-        <f>H53/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65345,15 +65341,15 @@
         <v>52</v>
       </c>
       <c r="G54">
-        <f>E54/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H54">
-        <f>LOG10(E54)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I54">
-        <f>H54/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65374,15 +65370,15 @@
         <v>53</v>
       </c>
       <c r="G55">
-        <f>E55/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H55">
-        <f>LOG10(E55)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I55">
-        <f>H55/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65403,15 +65399,15 @@
         <v>54</v>
       </c>
       <c r="G56">
-        <f>E56/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H56">
-        <f>LOG10(E56)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I56">
-        <f>H56/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65432,15 +65428,15 @@
         <v>55</v>
       </c>
       <c r="G57">
-        <f>E57/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H57">
-        <f>LOG10(E57)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I57">
-        <f>H57/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65461,15 +65457,15 @@
         <v>56</v>
       </c>
       <c r="G58">
-        <f>E58/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H58">
-        <f>LOG10(E58)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I58">
-        <f>H58/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65490,15 +65486,15 @@
         <v>57</v>
       </c>
       <c r="G59">
-        <f>E59/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H59">
-        <f>LOG10(E59)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I59">
-        <f>H59/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65519,15 +65515,15 @@
         <v>58</v>
       </c>
       <c r="G60">
-        <f>E60/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H60">
-        <f>LOG10(E60)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I60">
-        <f>H60/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>
@@ -65548,15 +65544,15 @@
         <v>59</v>
       </c>
       <c r="G61">
-        <f>E61/$E$3</f>
+        <f t="shared" si="3"/>
         <v>2.564102564102564E-2</v>
       </c>
       <c r="H61">
-        <f>LOG10(E61)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I61">
-        <f>H61/$H$3</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>